<commit_message>
[MS-ADMINS] Add new case and capture code for 2 fixed TDIs [MS-ADMINS] Add and update cases and capture code for latest RS
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-ADMINS/MS-ADMINS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-ADMINS/MS-ADMINS_RequirementSpecification.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$211</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="483">
   <si>
     <t>Req ID</t>
   </si>
@@ -1679,12 +1679,6 @@
     <t>MS-ADMINS_R18002</t>
   </si>
   <si>
-    <t>[In CreateSiteSoapIn]Otherwise, if the LCID is invalid [or not installed], then the server MUST return a SOAP fault with error code 0x8102005e.</t>
-  </si>
-  <si>
-    <t>[In CreateSiteSoapIn]Otherwise, if the LCID is [invalid or] not installed, then the server MUST return a SOAP fault with error code 0x8102005e.</t>
-  </si>
-  <si>
     <t xml:space="preserve">[In CreateSiteSoapIn] If the LCID is less than zero, server MUST create the site with current server language. </t>
   </si>
   <si>
@@ -1762,6 +1756,27 @@
        &lt;s:pattern value="[0-9a-fA-F]{8}-[0-9a-fA-F]{4}-[0-9a-fA-F]{4}-[0-9a-fA-F]{4}-[0-9a-fA-F]{12}" /&gt;
      &lt;/s:restriction&gt;
  &lt;/s:simpleType&gt;</t>
+  </si>
+  <si>
+    <t>[In CreateSiteSoapIn] If the LCID is invalid [or not installed], then the server MUST return a SOAP fault with error code 0x8102005e.</t>
+  </si>
+  <si>
+    <t>[In CreateSiteSoapIn] If the LCID is [invalid or] not installed, then the server MUST return a SOAP fault with error code 0x8102005e.</t>
+  </si>
+  <si>
+    <t>MS-ADMINS_R2042001</t>
+  </si>
+  <si>
+    <t>MS-ADMINS_R2042:c</t>
+  </si>
+  <si>
+    <t>MS-ADMINS_R2042002</t>
+  </si>
+  <si>
+    <t>[In CreateSite]PortNumber in the [Url's] first format [http://ServerName:PortNumber/sites/SiteCollectionName] MUST be the port number used by the web application  on the protocol server.</t>
+  </si>
+  <si>
+    <t>[In CreateSite]PortNumber in the [Url's] first format [http://ServerName:PortNumber/sites/SiteCollectionName] MUST be the port number used by or the Administration Web Service on the protocol server.</t>
   </si>
 </sst>
 </file>
@@ -2591,8 +2606,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I209" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I209"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I211" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I211"/>
   <tableColumns count="9">
     <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -2960,7 +2975,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L211"/>
+  <dimension ref="A1:L213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -5008,9 +5023,11 @@
       <c r="A88" s="22" t="s">
         <v>449</v>
       </c>
-      <c r="B88" s="31"/>
+      <c r="B88" s="31" t="s">
+        <v>235</v>
+      </c>
       <c r="C88" s="20" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D88" s="30"/>
       <c r="E88" s="30" t="s">
@@ -5020,10 +5037,10 @@
         <v>6</v>
       </c>
       <c r="G88" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H88" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I88" s="32"/>
     </row>
@@ -5035,7 +5052,7 @@
         <v>235</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>451</v>
+        <v>476</v>
       </c>
       <c r="D89" s="30"/>
       <c r="E89" s="30" t="s">
@@ -5060,7 +5077,7 @@
         <v>235</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>452</v>
+        <v>477</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="30" t="s">
@@ -5364,7 +5381,7 @@
         <v>237</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D102" s="30"/>
       <c r="E102" s="30" t="s">
@@ -5407,14 +5424,14 @@
       <c r="I103" s="32"/>
     </row>
     <row r="104" spans="1:9" ht="45">
-      <c r="A104" s="30" t="s">
+      <c r="A104" s="22" t="s">
         <v>126</v>
       </c>
       <c r="B104" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D104" s="30"/>
       <c r="E104" s="30" t="s">
@@ -5427,21 +5444,23 @@
         <v>15</v>
       </c>
       <c r="H104" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9">
-      <c r="A105" s="30" t="s">
-        <v>127</v>
+    <row r="105" spans="1:9" ht="45">
+      <c r="A105" s="22" t="s">
+        <v>478</v>
       </c>
       <c r="B105" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C105" s="32" t="s">
-        <v>334</v>
-      </c>
-      <c r="D105" s="30"/>
+      <c r="C105" s="20" t="s">
+        <v>481</v>
+      </c>
+      <c r="D105" s="22" t="s">
+        <v>479</v>
+      </c>
       <c r="E105" s="30" t="s">
         <v>19</v>
       </c>
@@ -5449,24 +5468,26 @@
         <v>3</v>
       </c>
       <c r="G105" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H105" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I105" s="32"/>
     </row>
-    <row r="106" spans="1:9" ht="60">
-      <c r="A106" s="30" t="s">
-        <v>128</v>
+    <row r="106" spans="1:9" ht="45">
+      <c r="A106" s="22" t="s">
+        <v>480</v>
       </c>
       <c r="B106" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C106" s="32" t="s">
-        <v>335</v>
-      </c>
-      <c r="D106" s="30"/>
+      <c r="C106" s="20" t="s">
+        <v>482</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>479</v>
+      </c>
       <c r="E106" s="30" t="s">
         <v>19</v>
       </c>
@@ -5477,25 +5498,21 @@
         <v>15</v>
       </c>
       <c r="H106" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I106" s="32" t="s">
-        <v>438</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I106" s="32"/>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B107" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C107" s="32" t="s">
-        <v>336</v>
-      </c>
-      <c r="D107" s="30" t="s">
-        <v>427</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="D107" s="30"/>
       <c r="E107" s="30" t="s">
         <v>19</v>
       </c>
@@ -5503,26 +5520,24 @@
         <v>3</v>
       </c>
       <c r="G107" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H107" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I107" s="32"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" ht="60">
       <c r="A108" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B108" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="D108" s="30" t="s">
-        <v>427</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="D108" s="30"/>
       <c r="E108" s="30" t="s">
         <v>19</v>
       </c>
@@ -5533,19 +5548,21 @@
         <v>15</v>
       </c>
       <c r="H108" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I108" s="32"/>
-    </row>
-    <row r="109" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I108" s="32" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109" s="30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B109" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D109" s="30" t="s">
         <v>427</v>
@@ -5566,15 +5583,17 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B110" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C110" s="32" t="s">
-        <v>339</v>
-      </c>
-      <c r="D110" s="30"/>
+        <v>337</v>
+      </c>
+      <c r="D110" s="30" t="s">
+        <v>427</v>
+      </c>
       <c r="E110" s="30" t="s">
         <v>19</v>
       </c>
@@ -5589,17 +5608,19 @@
       </c>
       <c r="I110" s="32"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" ht="30">
       <c r="A111" s="30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B111" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>340</v>
-      </c>
-      <c r="D111" s="30"/>
+        <v>338</v>
+      </c>
+      <c r="D111" s="30" t="s">
+        <v>427</v>
+      </c>
       <c r="E111" s="30" t="s">
         <v>19</v>
       </c>
@@ -5607,22 +5628,22 @@
         <v>3</v>
       </c>
       <c r="G111" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H111" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I111" s="32"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B112" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D112" s="30"/>
       <c r="E112" s="30" t="s">
@@ -5639,15 +5660,15 @@
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" ht="30">
+    <row r="113" spans="1:9">
       <c r="A113" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B113" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C113" s="32" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D113" s="30"/>
       <c r="E113" s="30" t="s">
@@ -5664,15 +5685,15 @@
       </c>
       <c r="I113" s="32"/>
     </row>
-    <row r="114" spans="1:9" ht="30">
+    <row r="114" spans="1:9">
       <c r="A114" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B114" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B114" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C114" s="20" t="s">
-        <v>343</v>
+      <c r="C114" s="32" t="s">
+        <v>341</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="30" t="s">
@@ -5685,21 +5706,19 @@
         <v>15</v>
       </c>
       <c r="H114" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I114" s="32" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
+        <v>20</v>
+      </c>
+      <c r="I114" s="32"/>
+    </row>
+    <row r="115" spans="1:9" ht="30">
       <c r="A115" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B115" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D115" s="30"/>
       <c r="E115" s="30" t="s">
@@ -5716,15 +5735,15 @@
       </c>
       <c r="I115" s="32"/>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" ht="30">
       <c r="A116" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="B116" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B116" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="C116" s="32" t="s">
-        <v>345</v>
+      <c r="C116" s="20" t="s">
+        <v>343</v>
       </c>
       <c r="D116" s="30"/>
       <c r="E116" s="30" t="s">
@@ -5734,22 +5753,24 @@
         <v>3</v>
       </c>
       <c r="G116" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H116" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I116" s="32"/>
-    </row>
-    <row r="117" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I116" s="32" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
       <c r="A117" s="30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B117" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D117" s="30"/>
       <c r="E117" s="30" t="s">
@@ -5759,7 +5780,7 @@
         <v>3</v>
       </c>
       <c r="G117" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H117" s="30" t="s">
         <v>18</v>
@@ -5768,13 +5789,13 @@
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B118" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D118" s="30"/>
       <c r="E118" s="30" t="s">
@@ -5791,15 +5812,15 @@
       </c>
       <c r="I118" s="32"/>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" ht="30">
       <c r="A119" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B119" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C119" s="32" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D119" s="30"/>
       <c r="E119" s="30" t="s">
@@ -5812,19 +5833,19 @@
         <v>15</v>
       </c>
       <c r="H119" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I119" s="32"/>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B120" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C120" s="20" t="s">
-        <v>349</v>
+      <c r="C120" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="D120" s="30"/>
       <c r="E120" s="30" t="s">
@@ -5834,22 +5855,22 @@
         <v>3</v>
       </c>
       <c r="G120" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H120" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I120" s="32"/>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="22" t="s">
-        <v>456</v>
+      <c r="A121" s="30" t="s">
+        <v>141</v>
       </c>
       <c r="B121" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C121" s="20" t="s">
-        <v>457</v>
+      <c r="C121" s="32" t="s">
+        <v>348</v>
       </c>
       <c r="D121" s="30"/>
       <c r="E121" s="30" t="s">
@@ -5862,19 +5883,19 @@
         <v>15</v>
       </c>
       <c r="H121" s="30" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I121" s="32"/>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B122" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C122" s="32" t="s">
-        <v>350</v>
+      <c r="C122" s="20" t="s">
+        <v>349</v>
       </c>
       <c r="D122" s="30"/>
       <c r="E122" s="30" t="s">
@@ -5884,22 +5905,22 @@
         <v>3</v>
       </c>
       <c r="G122" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H122" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9" ht="60">
-      <c r="A123" s="30" t="s">
-        <v>144</v>
+    <row r="123" spans="1:9">
+      <c r="A123" s="22" t="s">
+        <v>454</v>
       </c>
       <c r="B123" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C123" s="32" t="s">
-        <v>351</v>
+      <c r="C123" s="20" t="s">
+        <v>455</v>
       </c>
       <c r="D123" s="30"/>
       <c r="E123" s="30" t="s">
@@ -5912,25 +5933,21 @@
         <v>15</v>
       </c>
       <c r="H123" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I123" s="32" t="s">
-        <v>439</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I123" s="32"/>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B124" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>352</v>
-      </c>
-      <c r="D124" s="30" t="s">
-        <v>428</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="D124" s="30"/>
       <c r="E124" s="30" t="s">
         <v>19</v>
       </c>
@@ -5938,26 +5955,24 @@
         <v>3</v>
       </c>
       <c r="G124" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H124" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" ht="60">
       <c r="A125" s="30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B125" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C125" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="D125" s="30" t="s">
-        <v>428</v>
-      </c>
+        <v>351</v>
+      </c>
+      <c r="D125" s="30"/>
       <c r="E125" s="30" t="s">
         <v>19</v>
       </c>
@@ -5968,19 +5983,21 @@
         <v>15</v>
       </c>
       <c r="H125" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I125" s="32"/>
-    </row>
-    <row r="126" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I125" s="32" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
       <c r="A126" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B126" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C126" s="32" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D126" s="30" t="s">
         <v>428</v>
@@ -5999,17 +6016,19 @@
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" ht="30">
+    <row r="127" spans="1:9">
       <c r="A127" s="30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B127" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C127" s="32" t="s">
-        <v>355</v>
-      </c>
-      <c r="D127" s="30"/>
+        <v>353</v>
+      </c>
+      <c r="D127" s="30" t="s">
+        <v>428</v>
+      </c>
       <c r="E127" s="30" t="s">
         <v>19</v>
       </c>
@@ -6020,21 +6039,23 @@
         <v>15</v>
       </c>
       <c r="H127" s="30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I127" s="32"/>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" ht="30">
       <c r="A128" s="30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B128" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C128" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="D128" s="30"/>
+        <v>354</v>
+      </c>
+      <c r="D128" s="30" t="s">
+        <v>428</v>
+      </c>
       <c r="E128" s="30" t="s">
         <v>19</v>
       </c>
@@ -6042,22 +6063,22 @@
         <v>3</v>
       </c>
       <c r="G128" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H128" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I128" s="32"/>
     </row>
-    <row r="129" spans="1:9" ht="60">
+    <row r="129" spans="1:9" ht="30">
       <c r="A129" s="30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B129" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C129" s="32" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D129" s="30"/>
       <c r="E129" s="30" t="s">
@@ -6072,23 +6093,19 @@
       <c r="H129" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I129" s="32" t="s">
-        <v>440</v>
-      </c>
+      <c r="I129" s="32"/>
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B130" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C130" s="32" t="s">
-        <v>358</v>
-      </c>
-      <c r="D130" s="30" t="s">
-        <v>429</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="D130" s="30"/>
       <c r="E130" s="30" t="s">
         <v>19</v>
       </c>
@@ -6096,26 +6113,24 @@
         <v>3</v>
       </c>
       <c r="G130" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H130" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I130" s="32"/>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" ht="60">
       <c r="A131" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B131" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C131" s="32" t="s">
-        <v>359</v>
-      </c>
-      <c r="D131" s="30" t="s">
-        <v>429</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="D131" s="30"/>
       <c r="E131" s="30" t="s">
         <v>19</v>
       </c>
@@ -6126,19 +6141,21 @@
         <v>15</v>
       </c>
       <c r="H131" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I131" s="32"/>
-    </row>
-    <row r="132" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I131" s="32" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
       <c r="A132" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B132" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C132" s="32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D132" s="30" t="s">
         <v>429</v>
@@ -6157,17 +6174,19 @@
       </c>
       <c r="I132" s="32"/>
     </row>
-    <row r="133" spans="1:9" ht="30">
+    <row r="133" spans="1:9">
       <c r="A133" s="30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B133" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C133" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="D133" s="30"/>
+        <v>359</v>
+      </c>
+      <c r="D133" s="30" t="s">
+        <v>429</v>
+      </c>
       <c r="E133" s="30" t="s">
         <v>19</v>
       </c>
@@ -6178,21 +6197,23 @@
         <v>15</v>
       </c>
       <c r="H133" s="30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I133" s="32"/>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" ht="30">
       <c r="A134" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B134" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C134" s="32" t="s">
-        <v>362</v>
-      </c>
-      <c r="D134" s="30"/>
+        <v>360</v>
+      </c>
+      <c r="D134" s="30" t="s">
+        <v>429</v>
+      </c>
       <c r="E134" s="30" t="s">
         <v>19</v>
       </c>
@@ -6200,22 +6221,22 @@
         <v>3</v>
       </c>
       <c r="G134" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H134" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I134" s="32"/>
     </row>
-    <row r="135" spans="1:9" ht="60">
+    <row r="135" spans="1:9" ht="30">
       <c r="A135" s="30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B135" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C135" s="32" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D135" s="30"/>
       <c r="E135" s="30" t="s">
@@ -6230,23 +6251,19 @@
       <c r="H135" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I135" s="32" t="s">
-        <v>441</v>
-      </c>
+      <c r="I135" s="32"/>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B136" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C136" s="32" t="s">
-        <v>364</v>
-      </c>
-      <c r="D136" s="30" t="s">
-        <v>430</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="D136" s="30"/>
       <c r="E136" s="30" t="s">
         <v>19</v>
       </c>
@@ -6254,26 +6271,24 @@
         <v>3</v>
       </c>
       <c r="G136" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H136" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I136" s="32"/>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" ht="60">
       <c r="A137" s="30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B137" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C137" s="32" t="s">
-        <v>365</v>
-      </c>
-      <c r="D137" s="30" t="s">
-        <v>430</v>
-      </c>
+        <v>363</v>
+      </c>
+      <c r="D137" s="30"/>
       <c r="E137" s="30" t="s">
         <v>19</v>
       </c>
@@ -6284,19 +6299,21 @@
         <v>15</v>
       </c>
       <c r="H137" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I137" s="32"/>
-    </row>
-    <row r="138" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I137" s="32" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
       <c r="A138" s="30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B138" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C138" s="32" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D138" s="30" t="s">
         <v>430</v>
@@ -6317,15 +6334,17 @@
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B139" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C139" s="32" t="s">
-        <v>367</v>
-      </c>
-      <c r="D139" s="30"/>
+        <v>365</v>
+      </c>
+      <c r="D139" s="30" t="s">
+        <v>430</v>
+      </c>
       <c r="E139" s="30" t="s">
         <v>19</v>
       </c>
@@ -6342,15 +6361,17 @@
     </row>
     <row r="140" spans="1:9" ht="30">
       <c r="A140" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B140" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C140" s="32" t="s">
-        <v>368</v>
-      </c>
-      <c r="D140" s="30"/>
+        <v>366</v>
+      </c>
+      <c r="D140" s="30" t="s">
+        <v>430</v>
+      </c>
       <c r="E140" s="30" t="s">
         <v>19</v>
       </c>
@@ -6358,22 +6379,22 @@
         <v>3</v>
       </c>
       <c r="G140" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H140" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I140" s="32"/>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="30" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B141" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C141" s="32" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D141" s="30"/>
       <c r="E141" s="30" t="s">
@@ -6390,15 +6411,15 @@
       </c>
       <c r="I141" s="32"/>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" ht="30">
       <c r="A142" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B142" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C142" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D142" s="30"/>
       <c r="E142" s="30" t="s">
@@ -6415,15 +6436,15 @@
       </c>
       <c r="I142" s="32"/>
     </row>
-    <row r="143" spans="1:9" ht="60">
+    <row r="143" spans="1:9">
       <c r="A143" s="30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B143" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C143" s="32" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D143" s="30"/>
       <c r="E143" s="30" t="s">
@@ -6436,25 +6457,21 @@
         <v>15</v>
       </c>
       <c r="H143" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I143" s="32" t="s">
-        <v>442</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I143" s="32"/>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B144" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C144" s="32" t="s">
-        <v>372</v>
-      </c>
-      <c r="D144" s="30" t="s">
-        <v>431</v>
-      </c>
+        <v>370</v>
+      </c>
+      <c r="D144" s="30"/>
       <c r="E144" s="30" t="s">
         <v>19</v>
       </c>
@@ -6462,26 +6479,24 @@
         <v>3</v>
       </c>
       <c r="G144" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H144" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I144" s="32"/>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" ht="60">
       <c r="A145" s="30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B145" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C145" s="32" t="s">
-        <v>373</v>
-      </c>
-      <c r="D145" s="30" t="s">
-        <v>431</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="D145" s="30"/>
       <c r="E145" s="30" t="s">
         <v>19</v>
       </c>
@@ -6492,19 +6507,21 @@
         <v>15</v>
       </c>
       <c r="H145" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I145" s="32"/>
-    </row>
-    <row r="146" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I145" s="32" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
       <c r="A146" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B146" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C146" s="32" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D146" s="30" t="s">
         <v>431</v>
@@ -6525,15 +6542,17 @@
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B147" s="31" t="s">
         <v>237</v>
       </c>
       <c r="C147" s="32" t="s">
-        <v>375</v>
-      </c>
-      <c r="D147" s="30"/>
+        <v>373</v>
+      </c>
+      <c r="D147" s="30" t="s">
+        <v>431</v>
+      </c>
       <c r="E147" s="30" t="s">
         <v>19</v>
       </c>
@@ -6550,63 +6569,65 @@
     </row>
     <row r="148" spans="1:9" ht="30">
       <c r="A148" s="30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B148" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C148" s="32" t="s">
-        <v>376</v>
-      </c>
-      <c r="D148" s="30"/>
+        <v>374</v>
+      </c>
+      <c r="D148" s="30" t="s">
+        <v>431</v>
+      </c>
       <c r="E148" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F148" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G148" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H148" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I148" s="32"/>
     </row>
-    <row r="149" spans="1:9" ht="120">
+    <row r="149" spans="1:9">
       <c r="A149" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C149" s="32" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D149" s="30"/>
       <c r="E149" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F149" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G149" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H149" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I149" s="32"/>
     </row>
-    <row r="150" spans="1:9">
-      <c r="A150" s="22" t="s">
-        <v>171</v>
+    <row r="150" spans="1:9" ht="30">
+      <c r="A150" s="30" t="s">
+        <v>169</v>
       </c>
       <c r="B150" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="C150" s="20" t="s">
-        <v>378</v>
+      <c r="C150" s="32" t="s">
+        <v>376</v>
       </c>
       <c r="D150" s="30"/>
       <c r="E150" s="30" t="s">
@@ -6616,22 +6637,22 @@
         <v>6</v>
       </c>
       <c r="G150" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H150" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I150" s="32"/>
     </row>
-    <row r="151" spans="1:9">
-      <c r="A151" s="22" t="s">
-        <v>458</v>
+    <row r="151" spans="1:9" ht="120">
+      <c r="A151" s="30" t="s">
+        <v>170</v>
       </c>
       <c r="B151" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="C151" s="20" t="s">
-        <v>459</v>
+      <c r="C151" s="32" t="s">
+        <v>377</v>
       </c>
       <c r="D151" s="30"/>
       <c r="E151" s="30" t="s">
@@ -6644,69 +6665,69 @@
         <v>15</v>
       </c>
       <c r="H151" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I151" s="32"/>
     </row>
     <row r="152" spans="1:9">
-      <c r="A152" s="30" t="s">
-        <v>172</v>
+      <c r="A152" s="22" t="s">
+        <v>171</v>
       </c>
       <c r="B152" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C152" s="32" t="s">
-        <v>379</v>
+        <v>238</v>
+      </c>
+      <c r="C152" s="20" t="s">
+        <v>378</v>
       </c>
       <c r="D152" s="30"/>
       <c r="E152" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F152" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G152" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H152" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I152" s="32"/>
     </row>
-    <row r="153" spans="1:9" ht="60">
-      <c r="A153" s="30" t="s">
-        <v>173</v>
+    <row r="153" spans="1:9">
+      <c r="A153" s="22" t="s">
+        <v>456</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C153" s="32" t="s">
-        <v>380</v>
+        <v>238</v>
+      </c>
+      <c r="C153" s="20" t="s">
+        <v>457</v>
       </c>
       <c r="D153" s="30"/>
       <c r="E153" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F153" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G153" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H153" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I153" s="32"/>
     </row>
-    <row r="154" spans="1:9" ht="30">
+    <row r="154" spans="1:9">
       <c r="A154" s="30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B154" s="31" t="s">
         <v>33</v>
       </c>
       <c r="C154" s="32" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D154" s="30"/>
       <c r="E154" s="30" t="s">
@@ -6716,22 +6737,22 @@
         <v>3</v>
       </c>
       <c r="G154" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H154" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I154" s="32"/>
     </row>
-    <row r="155" spans="1:9" ht="30">
+    <row r="155" spans="1:9" ht="60">
       <c r="A155" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B155" s="31" t="s">
         <v>33</v>
       </c>
       <c r="C155" s="32" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D155" s="30"/>
       <c r="E155" s="30" t="s">
@@ -6744,69 +6765,69 @@
         <v>15</v>
       </c>
       <c r="H155" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I155" s="32"/>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" ht="30">
       <c r="A156" s="30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>239</v>
+        <v>33</v>
       </c>
       <c r="C156" s="32" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D156" s="30"/>
       <c r="E156" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F156" s="30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G156" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H156" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I156" s="32"/>
     </row>
     <row r="157" spans="1:9" ht="30">
       <c r="A157" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B157" s="31" t="s">
-        <v>239</v>
+        <v>33</v>
       </c>
       <c r="C157" s="32" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D157" s="30"/>
       <c r="E157" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F157" s="30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G157" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H157" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I157" s="32"/>
     </row>
     <row r="158" spans="1:9">
       <c r="A158" s="30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B158" s="31" t="s">
         <v>239</v>
       </c>
       <c r="C158" s="32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D158" s="30"/>
       <c r="E158" s="30" t="s">
@@ -6825,70 +6846,70 @@
     </row>
     <row r="159" spans="1:9" ht="30">
       <c r="A159" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B159" s="31" t="s">
         <v>239</v>
       </c>
       <c r="C159" s="32" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D159" s="30"/>
       <c r="E159" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F159" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G159" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H159" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I159" s="32"/>
     </row>
-    <row r="160" spans="1:9" ht="30">
+    <row r="160" spans="1:9">
       <c r="A160" s="30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B160" s="31" t="s">
         <v>239</v>
       </c>
       <c r="C160" s="32" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D160" s="30"/>
       <c r="E160" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F160" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G160" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H160" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I160" s="32"/>
     </row>
     <row r="161" spans="1:9" ht="30">
       <c r="A161" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B161" s="31" t="s">
         <v>239</v>
       </c>
       <c r="C161" s="32" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D161" s="30"/>
       <c r="E161" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F161" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G161" s="30" t="s">
         <v>15</v>
@@ -6900,13 +6921,13 @@
     </row>
     <row r="162" spans="1:9" ht="30">
       <c r="A162" s="30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B162" s="31" t="s">
         <v>239</v>
       </c>
       <c r="C162" s="32" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D162" s="30"/>
       <c r="E162" s="30" t="s">
@@ -6925,13 +6946,13 @@
     </row>
     <row r="163" spans="1:9" ht="30">
       <c r="A163" s="30" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B163" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C163" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D163" s="30"/>
       <c r="E163" s="30" t="s">
@@ -6941,22 +6962,22 @@
         <v>6</v>
       </c>
       <c r="G163" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H163" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I163" s="32"/>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" ht="30">
       <c r="A164" s="30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B164" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C164" s="32" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D164" s="30"/>
       <c r="E164" s="30" t="s">
@@ -6969,26 +6990,26 @@
         <v>15</v>
       </c>
       <c r="H164" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I164" s="32"/>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" ht="30">
       <c r="A165" s="30" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B165" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C165" s="32" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D165" s="30"/>
       <c r="E165" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F165" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G165" s="30" t="s">
         <v>16</v>
@@ -6998,47 +7019,47 @@
       </c>
       <c r="I165" s="32"/>
     </row>
-    <row r="166" spans="1:9" ht="105">
+    <row r="166" spans="1:9">
       <c r="A166" s="30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B166" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C166" s="32" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D166" s="30"/>
       <c r="E166" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F166" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G166" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H166" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I166" s="32"/>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" s="30" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B167" s="31" t="s">
         <v>241</v>
       </c>
       <c r="C167" s="32" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D167" s="30"/>
       <c r="E167" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F167" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G167" s="30" t="s">
         <v>16</v>
@@ -7048,72 +7069,72 @@
       </c>
       <c r="I167" s="32"/>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" ht="105">
       <c r="A168" s="30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B168" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C168" s="32" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D168" s="30"/>
       <c r="E168" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F168" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G168" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H168" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I168" s="32"/>
     </row>
-    <row r="169" spans="1:9" ht="30">
+    <row r="169" spans="1:9">
       <c r="A169" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B169" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C169" s="32" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D169" s="30"/>
       <c r="E169" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F169" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G169" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H169" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I169" s="32"/>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" s="30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B170" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C170" s="32" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D170" s="30"/>
       <c r="E170" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F170" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G170" s="30" t="s">
         <v>16</v>
@@ -7123,22 +7144,22 @@
       </c>
       <c r="I170" s="32"/>
     </row>
-    <row r="171" spans="1:9" ht="75">
+    <row r="171" spans="1:9" ht="30">
       <c r="A171" s="30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B171" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C171" s="32" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D171" s="30"/>
       <c r="E171" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F171" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G171" s="30" t="s">
         <v>15</v>
@@ -7148,90 +7169,90 @@
       </c>
       <c r="I171" s="32"/>
     </row>
-    <row r="172" spans="1:9" ht="30">
+    <row r="172" spans="1:9">
       <c r="A172" s="30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B172" s="31" t="s">
         <v>243</v>
       </c>
       <c r="C172" s="32" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D172" s="30"/>
       <c r="E172" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F172" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G172" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H172" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I172" s="32"/>
     </row>
-    <row r="173" spans="1:9" ht="30">
+    <row r="173" spans="1:9" ht="75">
       <c r="A173" s="30" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B173" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C173" s="32" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D173" s="30"/>
       <c r="E173" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F173" s="30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G173" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H173" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I173" s="32"/>
     </row>
     <row r="174" spans="1:9" ht="30">
       <c r="A174" s="30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B174" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C174" s="32" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D174" s="30"/>
       <c r="E174" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F174" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G174" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H174" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I174" s="32"/>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" ht="30">
       <c r="A175" s="30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B175" s="31" t="s">
         <v>244</v>
       </c>
       <c r="C175" s="32" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D175" s="30"/>
       <c r="E175" s="30" t="s">
@@ -7241,32 +7262,32 @@
         <v>7</v>
       </c>
       <c r="G175" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H175" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I175" s="32"/>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" ht="30">
       <c r="A176" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B176" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C176" s="32" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D176" s="30"/>
       <c r="E176" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F176" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G176" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H176" s="30" t="s">
         <v>18</v>
@@ -7275,45 +7296,45 @@
     </row>
     <row r="177" spans="1:9">
       <c r="A177" s="30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B177" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C177" s="32" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D177" s="30"/>
       <c r="E177" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F177" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G177" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H177" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I177" s="32"/>
     </row>
-    <row r="178" spans="1:9" ht="30">
+    <row r="178" spans="1:9">
       <c r="A178" s="30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B178" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C178" s="32" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D178" s="30"/>
       <c r="E178" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F178" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G178" s="30" t="s">
         <v>16</v>
@@ -7323,47 +7344,47 @@
       </c>
       <c r="I178" s="32"/>
     </row>
-    <row r="179" spans="1:9" ht="45">
+    <row r="179" spans="1:9">
       <c r="A179" s="30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B179" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C179" s="32" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D179" s="30"/>
       <c r="E179" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F179" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G179" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H179" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I179" s="32"/>
     </row>
     <row r="180" spans="1:9" ht="30">
       <c r="A180" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B180" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C180" s="32" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D180" s="30"/>
       <c r="E180" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F180" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G180" s="30" t="s">
         <v>16</v>
@@ -7373,40 +7394,40 @@
       </c>
       <c r="I180" s="32"/>
     </row>
-    <row r="181" spans="1:9" ht="300">
+    <row r="181" spans="1:9" ht="45">
       <c r="A181" s="30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B181" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C181" s="32" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D181" s="30"/>
       <c r="E181" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F181" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G181" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H181" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I181" s="32"/>
     </row>
     <row r="182" spans="1:9" ht="30">
-      <c r="A182" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="B182" s="24" t="s">
+      <c r="A182" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="B182" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="C182" s="20" t="s">
-        <v>409</v>
+      <c r="C182" s="32" t="s">
+        <v>407</v>
       </c>
       <c r="D182" s="30"/>
       <c r="E182" s="30" t="s">
@@ -7416,22 +7437,22 @@
         <v>6</v>
       </c>
       <c r="G182" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H182" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I182" s="32"/>
     </row>
-    <row r="183" spans="1:9">
-      <c r="A183" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="B183" s="24" t="s">
+    <row r="183" spans="1:9" ht="300">
+      <c r="A183" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="B183" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="C183" s="20" t="s">
-        <v>461</v>
+      <c r="C183" s="32" t="s">
+        <v>408</v>
       </c>
       <c r="D183" s="30"/>
       <c r="E183" s="30" t="s">
@@ -7448,15 +7469,15 @@
       </c>
       <c r="I183" s="32"/>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" ht="30">
       <c r="A184" s="22" t="s">
-        <v>462</v>
+        <v>202</v>
       </c>
       <c r="B184" s="24" t="s">
         <v>247</v>
       </c>
       <c r="C184" s="20" t="s">
-        <v>463</v>
+        <v>409</v>
       </c>
       <c r="D184" s="30"/>
       <c r="E184" s="30" t="s">
@@ -7474,64 +7495,64 @@
       <c r="I184" s="32"/>
     </row>
     <row r="185" spans="1:9">
-      <c r="A185" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="B185" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="C185" s="32" t="s">
-        <v>410</v>
+      <c r="A185" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="B185" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C185" s="20" t="s">
+        <v>459</v>
       </c>
       <c r="D185" s="30"/>
       <c r="E185" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F185" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G185" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H185" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I185" s="32"/>
     </row>
     <row r="186" spans="1:9">
-      <c r="A186" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="B186" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="C186" s="32" t="s">
-        <v>411</v>
+      <c r="A186" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="B186" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C186" s="20" t="s">
+        <v>461</v>
       </c>
       <c r="D186" s="30"/>
       <c r="E186" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F186" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G186" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H186" s="30" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I186" s="32"/>
     </row>
-    <row r="187" spans="1:9" ht="75">
+    <row r="187" spans="1:9">
       <c r="A187" s="30" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B187" s="31" t="s">
         <v>248</v>
       </c>
       <c r="C187" s="32" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D187" s="30"/>
       <c r="E187" s="30" t="s">
@@ -7541,29 +7562,29 @@
         <v>3</v>
       </c>
       <c r="G187" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H187" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I187" s="32"/>
     </row>
-    <row r="188" spans="1:9" ht="30">
+    <row r="188" spans="1:9">
       <c r="A188" s="30" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B188" s="31" t="s">
         <v>248</v>
       </c>
       <c r="C188" s="32" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D188" s="30"/>
       <c r="E188" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F188" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G188" s="30" t="s">
         <v>15</v>
@@ -7573,65 +7594,65 @@
       </c>
       <c r="I188" s="32"/>
     </row>
-    <row r="189" spans="1:9" ht="30">
+    <row r="189" spans="1:9" ht="75">
       <c r="A189" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B189" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C189" s="32" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D189" s="30"/>
       <c r="E189" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F189" s="30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G189" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H189" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I189" s="32"/>
     </row>
-    <row r="190" spans="1:9" ht="45">
+    <row r="190" spans="1:9" ht="30">
       <c r="A190" s="30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B190" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C190" s="32" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D190" s="30"/>
       <c r="E190" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F190" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G190" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H190" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I190" s="32"/>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" ht="30">
       <c r="A191" s="30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B191" s="31" t="s">
         <v>249</v>
       </c>
       <c r="C191" s="32" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D191" s="30"/>
       <c r="E191" s="30" t="s">
@@ -7641,32 +7662,32 @@
         <v>7</v>
       </c>
       <c r="G191" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H191" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I191" s="32"/>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" ht="45">
       <c r="A192" s="30" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B192" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C192" s="32" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D192" s="30"/>
       <c r="E192" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F192" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G192" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H192" s="30" t="s">
         <v>18</v>
@@ -7675,45 +7696,45 @@
     </row>
     <row r="193" spans="1:9">
       <c r="A193" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B193" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C193" s="32" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D193" s="30"/>
       <c r="E193" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F193" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G193" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H193" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I193" s="32"/>
     </row>
     <row r="194" spans="1:9">
       <c r="A194" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B194" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C194" s="32" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D194" s="30"/>
       <c r="E194" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F194" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G194" s="30" t="s">
         <v>16</v>
@@ -7723,40 +7744,40 @@
       </c>
       <c r="I194" s="32"/>
     </row>
-    <row r="195" spans="1:9" ht="135">
+    <row r="195" spans="1:9">
       <c r="A195" s="30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B195" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C195" s="32" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D195" s="30"/>
       <c r="E195" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F195" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G195" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H195" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I195" s="32"/>
     </row>
     <row r="196" spans="1:9">
-      <c r="A196" s="22" t="s">
-        <v>214</v>
+      <c r="A196" s="30" t="s">
+        <v>212</v>
       </c>
       <c r="B196" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="C196" s="20" t="s">
-        <v>464</v>
+      <c r="C196" s="32" t="s">
+        <v>419</v>
       </c>
       <c r="D196" s="30"/>
       <c r="E196" s="30" t="s">
@@ -7766,22 +7787,22 @@
         <v>7</v>
       </c>
       <c r="G196" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H196" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I196" s="32"/>
     </row>
-    <row r="197" spans="1:9">
-      <c r="A197" s="22" t="s">
-        <v>465</v>
+    <row r="197" spans="1:9" ht="135">
+      <c r="A197" s="30" t="s">
+        <v>213</v>
       </c>
       <c r="B197" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="C197" s="20" t="s">
-        <v>466</v>
+      <c r="C197" s="32" t="s">
+        <v>420</v>
       </c>
       <c r="D197" s="30"/>
       <c r="E197" s="30" t="s">
@@ -7798,15 +7819,15 @@
       </c>
       <c r="I197" s="32"/>
     </row>
-    <row r="198" spans="1:9" ht="30">
-      <c r="A198" s="30" t="s">
-        <v>215</v>
+    <row r="198" spans="1:9">
+      <c r="A198" s="22" t="s">
+        <v>214</v>
       </c>
       <c r="B198" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="C198" s="32" t="s">
-        <v>421</v>
+      <c r="C198" s="20" t="s">
+        <v>462</v>
       </c>
       <c r="D198" s="30"/>
       <c r="E198" s="30" t="s">
@@ -7824,71 +7845,71 @@
       <c r="I198" s="32"/>
     </row>
     <row r="199" spans="1:9">
-      <c r="A199" s="30" t="s">
-        <v>216</v>
+      <c r="A199" s="22" t="s">
+        <v>463</v>
       </c>
       <c r="B199" s="31" t="s">
-        <v>252</v>
-      </c>
-      <c r="C199" s="32" t="s">
-        <v>422</v>
+        <v>251</v>
+      </c>
+      <c r="C199" s="20" t="s">
+        <v>464</v>
       </c>
       <c r="D199" s="30"/>
       <c r="E199" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F199" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G199" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H199" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I199" s="32"/>
     </row>
-    <row r="200" spans="1:9" ht="60">
-      <c r="A200" s="22" t="s">
-        <v>217</v>
+    <row r="200" spans="1:9" ht="30">
+      <c r="A200" s="30" t="s">
+        <v>215</v>
       </c>
       <c r="B200" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C200" s="32" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D200" s="30"/>
       <c r="E200" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F200" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G200" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H200" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I200" s="32"/>
     </row>
-    <row r="201" spans="1:9" ht="30">
-      <c r="A201" s="22" t="s">
-        <v>468</v>
-      </c>
-      <c r="B201" s="24" t="s">
-        <v>469</v>
-      </c>
-      <c r="C201" s="20" t="s">
-        <v>470</v>
+    <row r="201" spans="1:9">
+      <c r="A201" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="B201" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="C201" s="32" t="s">
+        <v>422</v>
       </c>
       <c r="D201" s="30"/>
       <c r="E201" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F201" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G201" s="30" t="s">
         <v>16</v>
@@ -7898,173 +7919,171 @@
       </c>
       <c r="I201" s="32"/>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" ht="60">
       <c r="A202" s="22" t="s">
-        <v>471</v>
-      </c>
-      <c r="B202" s="24" t="s">
-        <v>469</v>
-      </c>
-      <c r="C202" s="20" t="s">
-        <v>472</v>
+        <v>217</v>
+      </c>
+      <c r="B202" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="C202" s="32" t="s">
+        <v>423</v>
       </c>
       <c r="D202" s="30"/>
       <c r="E202" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F202" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G202" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H202" s="30" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I202" s="32"/>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" ht="30">
       <c r="A203" s="22" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B203" s="24" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="C203" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="D203" s="30"/>
       <c r="E203" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F203" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G203" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H203" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I203" s="32"/>
     </row>
-    <row r="204" spans="1:9" ht="75">
+    <row r="204" spans="1:9">
       <c r="A204" s="22" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="B204" s="24" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="C204" s="20" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="D204" s="30"/>
       <c r="E204" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F204" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G204" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H204" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I204" s="32"/>
     </row>
-    <row r="205" spans="1:9" s="23" customFormat="1" ht="45">
+    <row r="205" spans="1:9">
       <c r="A205" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B205" s="33">
+        <v>471</v>
+      </c>
+      <c r="B205" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="C205" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="D205" s="30"/>
+      <c r="E205" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F205" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C205" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="D205" s="22" t="s">
-        <v>424</v>
-      </c>
-      <c r="E205" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F205" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G205" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H205" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I205" s="24" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" ht="45">
-      <c r="A206" s="30" t="s">
-        <v>218</v>
-      </c>
-      <c r="B206" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="C206" s="32" t="s">
-        <v>445</v>
+      <c r="G205" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H205" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I205" s="32"/>
+    </row>
+    <row r="206" spans="1:9" ht="75">
+      <c r="A206" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="B206" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="C206" s="20" t="s">
+        <v>475</v>
       </c>
       <c r="D206" s="30"/>
       <c r="E206" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F206" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G206" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H206" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I206" s="32"/>
+    </row>
+    <row r="207" spans="1:9" s="23" customFormat="1" ht="45">
+      <c r="A207" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B207" s="33">
+        <v>7</v>
+      </c>
+      <c r="C207" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="D207" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="E207" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F206" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G206" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="H206" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I206" s="32"/>
-    </row>
-    <row r="207" spans="1:9" ht="30">
-      <c r="A207" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="B207" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="C207" s="32" t="s">
-        <v>446</v>
-      </c>
-      <c r="D207" s="30"/>
-      <c r="E207" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F207" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G207" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="H207" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I207" s="32"/>
+      <c r="F207" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G207" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H207" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I207" s="24" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="208" spans="1:9" ht="45">
       <c r="A208" s="30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B208" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="C208" s="20" t="s">
-        <v>444</v>
-      </c>
-      <c r="D208" s="24" t="s">
-        <v>443</v>
-      </c>
+      <c r="C208" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="D208" s="30"/>
       <c r="E208" s="30" t="s">
         <v>22</v>
       </c>
@@ -8072,47 +8091,99 @@
         <v>3</v>
       </c>
       <c r="G208" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H208" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I208" s="32" t="s">
-        <v>432</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I208" s="32"/>
     </row>
     <row r="209" spans="1:9" ht="30">
       <c r="A209" s="30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B209" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="C209" s="20" t="s">
-        <v>467</v>
+      <c r="C209" s="32" t="s">
+        <v>446</v>
       </c>
       <c r="D209" s="30"/>
       <c r="E209" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F209" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G209" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H209" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I209" s="32"/>
+    </row>
+    <row r="210" spans="1:9" ht="45">
+      <c r="A210" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="B210" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="C210" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="D210" s="24" t="s">
+        <v>443</v>
+      </c>
+      <c r="E210" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F210" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G210" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H210" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I210" s="32" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" ht="30">
+      <c r="A211" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="B211" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="C211" s="20" t="s">
+        <v>465</v>
+      </c>
+      <c r="D211" s="30"/>
+      <c r="E211" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F211" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G209" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H209" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I209" s="32"/>
-    </row>
-    <row r="210" spans="1:9">
-      <c r="A210" s="3"/>
-      <c r="B210" s="10"/>
-    </row>
-    <row r="211" spans="1:9">
-      <c r="A211" s="3"/>
-      <c r="B211" s="10"/>
+      <c r="G211" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H211" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I211" s="32"/>
+    </row>
+    <row r="212" spans="1:9">
+      <c r="A212" s="3"/>
+      <c r="B212" s="10"/>
+    </row>
+    <row r="213" spans="1:9">
+      <c r="A213" s="3"/>
+      <c r="B213" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -8130,7 +8201,7 @@
     <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A206:I209 A20:I21 A205:H205 A22:H111 I22:I205 A33:I204">
+  <conditionalFormatting sqref="A208:I211 A20:I21 A207:H207 A22:H113 I22:I207 A33:I206">
     <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -8141,7 +8212,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A206:I209 A20:I21 A205:H205 A22:H111 I22:I205 A33:I204">
+  <conditionalFormatting sqref="A208:I211 A20:I21 A207:H207 A22:H113 I22:I207 A33:I206">
     <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -8152,7 +8223,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F209">
+  <conditionalFormatting sqref="F20:F211">
     <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
@@ -8161,20 +8232,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F209">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F211">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E209">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E211">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G209">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G211">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H209">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H211">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8184,7 +8255,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B2 B4:B9 B10:B21 B88:B90 B22:B87 B91:B184 B204:B211 B185:B203 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B2 B4:B9 B10:B21 B88:B90 B22:B87 B106:B186 B206:B213 B187:B205 B91:B105 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -8194,6 +8265,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -8242,22 +8322,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8272,7 +8351,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -8284,12 +8363,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-ADMINS: Update RS according to v20190618 document.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-ADMINS/MS-ADMINS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-ADMINS/MS-ADMINS_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F4DE3-1B8F-4C1A-B712-38733A681716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,8 +21,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmpF4C2" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmpF4C2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-zhalin\AppData\Local\Temp\tmpF4C2.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -1016,21 +1017,12 @@
     <t>[In Transport]Implementation does additionally support SOAP over HTTPS for securing communication with clients.(Windows SharePoint Services 3.0 and above products follow this behavior.)</t>
   </si>
   <si>
-    <t>[In Transport]Protocol messages MUST be formatted as specified either in [SOAP1.1], section 4 "SOAP Envelope" or in [SOAP1.2/1], section 5 "SOAP Message Construct."</t>
-  </si>
-  <si>
     <t>[In Transport]Protocol server faults MUST be returned using HTTP Status-Codes as specified in [RFC2616], section 10 "Status Code Definitions".</t>
   </si>
   <si>
-    <t>[In Transport]Protocol server faults MUST be returned using SOAP faults as specified either in [SOAP1.1], section 4.4 "SOAP Fault" or in [SOAP1.2/1], section 5.4 "SOAP Fault."</t>
-  </si>
-  <si>
     <t>[In Common Message Syntax]This section contains common definitions used by this protocol.</t>
   </si>
   <si>
-    <t>[In Common Message Syntax]The syntax of the definitions uses XML schema as defined in [XMLSCHEMA1] and [XMLSCHEMA2], and WSDL as defined in [WSDL].</t>
-  </si>
-  <si>
     <t>[In Namespaces]This protocol [MS-ADMINS] specifies and references XML namespaces using the mechanisms specified in [XMLNS].</t>
   </si>
   <si>
@@ -1041,12 +1033,6 @@
   </si>
   <si>
     <t>[In Namespaces]The Prefix "tns" is used for the namespace URI "http://schemas.microsoft.com/sharepoint/soap/".</t>
-  </si>
-  <si>
-    <t>[In Namespaces]The Prefix "s" is used for the namespace URI " http://www.w3.org/2001/XMLSchema", which refers to "[XMLSCHEMA1]" and "[XMLSCHEMA2]".</t>
-  </si>
-  <si>
-    <t>[In Namespaces]The Prefix "soap12" is used for the namespace URI "http://schemas.xmlsoap.org/wsdl/soap12/", which refers to "[SOAP1.2/1]" and "[SOAP1.2/2]".</t>
   </si>
   <si>
     <t>[In Namespaces]The Prefix "(none)" is used for the namespace URI "http://schemas.microsoft.com/sharepoint/soap/".</t>
@@ -1067,9 +1053,6 @@
   </si>
   <si>
     <t>[In Namespaces]The Prefix "http" is used for the namespace URI "http://schemas.xmlsoap.org/wsdl/http/", which refers to "[RFC2616]".</t>
-  </si>
-  <si>
-    <t>[In Namespaces]The Prefix "soapenc" is used for the namespace URI "http://schemas.xmlsoap.org/soap/encoding/", which refers to "[SOAP1.2/1]" and "[SOAP1.2/2]".</t>
   </si>
   <si>
     <t>[In Messages]This specification does not define any common WSDL message definitions.</t>
@@ -1125,9 +1108,6 @@
   </si>
   <si>
     <t>[In Protocol Details]This protocol [MS-ADMINS] allows protocol servers to notify protocol clients of application-level faults using SOAP faults.</t>
-  </si>
-  <si>
-    <t>[In Protocol Details]This protocol [MS-ADMINS] allows protocol servers to provide additional details for SOAP faults by including a detail element as specified either in [SOAP1.1], section 4.4 "SOAP Fault" or [SOAP1.2/1], section 5.4 "SOAP Fault" that conforms to the XML schema of the SOAPFaultDetails complex type specified in section 2.2.4.1.</t>
   </si>
   <si>
     <t>[In Protocol Details]Except where specified, these SOAP faults are not significant for interoperability, and protocol clients can interpret them in an implementation-specific manner.</t>
@@ -1673,13 +1653,7 @@
     <t>[Abstract Data Model]For an overview of site, site collection and site definition and protocol sever in general, see [MS-WSSTS] section 2.1.2.6 Site, [MS-WSSTS] section 2.1.2.5 Site Collection, and [MS-WSSTS] section 2.1.3.1 Site Definition.</t>
   </si>
   <si>
-    <t>MS-ADMINS_R18001</t>
-  </si>
-  <si>
     <t>MS-ADMINS_R18002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In CreateSiteSoapIn] If the LCID is less than zero, server MUST create the site with current server language. </t>
   </si>
   <si>
     <t>[In CreateSite]Its[Url's] maximum length, not including http://ServerName or http://ServerName:PortNumber, is 128 characters.</t>
@@ -1779,14 +1753,50 @@
     <t>[In CreateSite]PortNumber in the [Url's] first format [http://ServerName:PortNumber/sites/SiteCollectionName] MUST be the port number used by or the Administration Web Service on the protocol server.</t>
   </si>
   <si>
-    <t>5.0</t>
+    <t>7.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Transport]Protocol messages MUST be formatted as specified either in [SOAP1.1], section 4 "SOAP Envelope" or in [SOAP1.2-1/2007], section 5 "SOAP Message Construct."</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Transport]Protocol server faults MUST be returned using SOAP faults as specified either in [SOAP1.1], section 4.4 "SOAP Fault" or in [SOAP1.2-1/2007], section 5.4 "SOAP Fault."</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Common Message Syntax]The syntax of the definitions uses XML schema as defined in [XMLSCHEMA1/2] and [XMLSCHEMA2/2], and WSDL as defined in [WSDL].</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Namespaces]The Prefix "s" is used for the namespace URI " http://www.w3.org/2001/XMLSchema", which refers to "[XMLSCHEMA1/2]" and "[XMLSCHEMA2/2]".</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Namespaces]The Prefix "soap12" is used for the namespace URI "http://schemas.xmlsoap.org/wsdl/soap12/", which refers to "[SOAP1.2-1/2007]" and "[SOAP1.2-2/2007]".</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Namespaces]The Prefix "soapenc" is used for the namespace URI "http://schemas.xmlsoap.org/soap/encoding/", which refers to "[SOAP1.2-1/2007]" and "[SOAP1.2-2/2007]".</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Protocol Details]This protocol [MS-ADMINS] allows protocol servers to provide additional details for SOAP faults by including a detail element as specified either in [SOAP1.1], section 4.4 "SOAP Fault" or [SOAP1.2-1/2007], section 5.4 "SOAP Fault" that conforms to the XML schema of the SOAPFaultDetails complex type specified in section 2.2.4.1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In CreateSiteSoapIn] If the LCID is zero, the server MUST create the site with current server language. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-ADMINS_R18001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="177" formatCode="0.0.0"/>
@@ -2097,7 +2107,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
     <dxf>
@@ -2611,34 +2621,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I211" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I211"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I211" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I211" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2647,19 +2657,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2978,30 +2988,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.6328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.08984375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.7265625" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -3009,9 +3019,9 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3020,22 +3030,22 @@
       <c r="F2" s="25"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F3" s="12">
-        <v>42566</v>
+        <v>43634</v>
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
         <v>24</v>
       </c>
@@ -3047,7 +3057,7 @@
       <c r="G4" s="42"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
@@ -3063,7 +3073,7 @@
       <c r="I5" s="46"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
@@ -3079,7 +3089,7 @@
       <c r="I6" s="44"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -3095,7 +3105,7 @@
       <c r="I7" s="43"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
@@ -3111,7 +3121,7 @@
       <c r="I8" s="43"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
@@ -3127,7 +3137,7 @@
       <c r="I9" s="39"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
@@ -3143,7 +3153,7 @@
       <c r="I10" s="39"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
@@ -3159,7 +3169,7 @@
       <c r="I11" s="34"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
@@ -3177,7 +3187,7 @@
       <c r="I12" s="35"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
@@ -3195,7 +3205,7 @@
       <c r="I13" s="36"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
         <v>7</v>
       </c>
@@ -3213,7 +3223,7 @@
       <c r="I14" s="36"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
         <v>3</v>
       </c>
@@ -3231,7 +3241,7 @@
       <c r="I15" s="37"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
@@ -3247,7 +3257,7 @@
       <c r="I16" s="34"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -3263,7 +3273,7 @@
       <c r="I17" s="41"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -3280,7 +3290,7 @@
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -3310,7 +3320,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
@@ -3335,7 +3345,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>44</v>
       </c>
@@ -3359,10 +3369,10 @@
         <v>17</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>46</v>
       </c>
@@ -3370,7 +3380,7 @@
         <v>222</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>257</v>
+        <v>475</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
@@ -3387,7 +3397,7 @@
       </c>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>47</v>
       </c>
@@ -3395,7 +3405,7 @@
         <v>222</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="s">
@@ -3412,7 +3422,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>48</v>
       </c>
@@ -3420,7 +3430,7 @@
         <v>222</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>259</v>
+        <v>476</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="s">
@@ -3437,7 +3447,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>49</v>
       </c>
@@ -3445,7 +3455,7 @@
         <v>223</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -3462,7 +3472,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>50</v>
       </c>
@@ -3470,7 +3480,7 @@
         <v>223</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>261</v>
+        <v>477</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
@@ -3487,7 +3497,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -3495,7 +3505,7 @@
         <v>224</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22" t="s">
@@ -3512,7 +3522,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>52</v>
       </c>
@@ -3520,7 +3530,7 @@
         <v>224</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
@@ -3537,7 +3547,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>53</v>
       </c>
@@ -3545,7 +3555,7 @@
         <v>224</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22" t="s">
@@ -3562,7 +3572,7 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>54</v>
       </c>
@@ -3570,7 +3580,7 @@
         <v>224</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -3587,7 +3597,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>55</v>
       </c>
@@ -3595,7 +3605,7 @@
         <v>224</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>266</v>
+        <v>478</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22" t="s">
@@ -3612,7 +3622,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>56</v>
       </c>
@@ -3620,7 +3630,7 @@
         <v>224</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>267</v>
+        <v>479</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -3637,7 +3647,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="29" t="s">
         <v>57</v>
       </c>
@@ -3645,7 +3655,7 @@
         <v>224</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="29" t="s">
@@ -3662,7 +3672,7 @@
       </c>
       <c r="I33" s="31"/>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="29" t="s">
         <v>58</v>
       </c>
@@ -3670,7 +3680,7 @@
         <v>224</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29" t="s">
@@ -3687,7 +3697,7 @@
       </c>
       <c r="I34" s="31"/>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="29" t="s">
         <v>59</v>
       </c>
@@ -3695,7 +3705,7 @@
         <v>224</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29" t="s">
@@ -3712,7 +3722,7 @@
       </c>
       <c r="I35" s="31"/>
     </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="29" t="s">
         <v>60</v>
       </c>
@@ -3720,7 +3730,7 @@
         <v>224</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29" t="s">
@@ -3737,7 +3747,7 @@
       </c>
       <c r="I36" s="31"/>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="29" t="s">
         <v>61</v>
       </c>
@@ -3745,7 +3755,7 @@
         <v>224</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
@@ -3762,7 +3772,7 @@
       </c>
       <c r="I37" s="31"/>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="29" t="s">
         <v>62</v>
       </c>
@@ -3770,7 +3780,7 @@
         <v>224</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29" t="s">
@@ -3787,15 +3797,15 @@
       </c>
       <c r="I38" s="31"/>
     </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="29" t="s">
         <v>63</v>
       </c>
       <c r="B39" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="C39" s="31" t="s">
-        <v>274</v>
+      <c r="C39" s="20" t="s">
+        <v>480</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29" t="s">
@@ -3812,7 +3822,7 @@
       </c>
       <c r="I39" s="31"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="29" t="s">
         <v>64</v>
       </c>
@@ -3820,7 +3830,7 @@
         <v>225</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29" t="s">
@@ -3837,7 +3847,7 @@
       </c>
       <c r="I40" s="31"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="29" t="s">
         <v>65</v>
       </c>
@@ -3845,7 +3855,7 @@
         <v>226</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29" t="s">
@@ -3862,7 +3872,7 @@
       </c>
       <c r="I41" s="31"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="29" t="s">
         <v>66</v>
       </c>
@@ -3870,7 +3880,7 @@
         <v>31</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29" t="s">
@@ -3887,7 +3897,7 @@
       </c>
       <c r="I42" s="31"/>
     </row>
-    <row r="43" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A43" s="29" t="s">
         <v>67</v>
       </c>
@@ -3895,7 +3905,7 @@
         <v>31</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -3912,7 +3922,7 @@
       </c>
       <c r="I43" s="31"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="29" t="s">
         <v>68</v>
       </c>
@@ -3920,7 +3930,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29" t="s">
@@ -3937,7 +3947,7 @@
       </c>
       <c r="I44" s="31"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="29" t="s">
         <v>69</v>
       </c>
@@ -3945,7 +3955,7 @@
         <v>31</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29" t="s">
@@ -3962,7 +3972,7 @@
       </c>
       <c r="I45" s="31"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="29" t="s">
         <v>70</v>
       </c>
@@ -3970,7 +3980,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29" t="s">
@@ -3987,7 +3997,7 @@
       </c>
       <c r="I46" s="31"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="29" t="s">
         <v>71</v>
       </c>
@@ -3995,7 +4005,7 @@
         <v>227</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29" t="s">
@@ -4012,7 +4022,7 @@
       </c>
       <c r="I47" s="31"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="29" t="s">
         <v>72</v>
       </c>
@@ -4020,7 +4030,7 @@
         <v>228</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29" t="s">
@@ -4037,7 +4047,7 @@
       </c>
       <c r="I48" s="31"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="29" t="s">
         <v>73</v>
       </c>
@@ -4045,7 +4055,7 @@
         <v>229</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29" t="s">
@@ -4062,7 +4072,7 @@
       </c>
       <c r="I49" s="31"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="29" t="s">
         <v>74</v>
       </c>
@@ -4070,7 +4080,7 @@
         <v>230</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="29" t="s">
@@ -4087,7 +4097,7 @@
       </c>
       <c r="I50" s="31"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="29" t="s">
         <v>75</v>
       </c>
@@ -4095,7 +4105,7 @@
         <v>231</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="29" t="s">
@@ -4112,7 +4122,7 @@
       </c>
       <c r="I51" s="31"/>
     </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="29" t="s">
         <v>76</v>
       </c>
@@ -4120,7 +4130,7 @@
         <v>231</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D52" s="29"/>
       <c r="E52" s="29" t="s">
@@ -4137,7 +4147,7 @@
       </c>
       <c r="I52" s="31"/>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="29" t="s">
         <v>77</v>
       </c>
@@ -4145,7 +4155,7 @@
         <v>231</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="29" t="s">
@@ -4162,7 +4172,7 @@
       </c>
       <c r="I53" s="31"/>
     </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="29" t="s">
         <v>78</v>
       </c>
@@ -4170,7 +4180,7 @@
         <v>231</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D54" s="29"/>
       <c r="E54" s="29" t="s">
@@ -4187,7 +4197,7 @@
       </c>
       <c r="I54" s="31"/>
     </row>
-    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="29" t="s">
         <v>79</v>
       </c>
@@ -4195,7 +4205,7 @@
         <v>231</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29" t="s">
@@ -4212,15 +4222,15 @@
       </c>
       <c r="I55" s="31"/>
     </row>
-    <row r="56" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" s="29" t="s">
         <v>80</v>
       </c>
       <c r="B56" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="C56" s="31" t="s">
-        <v>291</v>
+      <c r="C56" s="20" t="s">
+        <v>481</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="29" t="s">
@@ -4237,7 +4247,7 @@
       </c>
       <c r="I56" s="31"/>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="29" t="s">
         <v>81</v>
       </c>
@@ -4245,7 +4255,7 @@
         <v>231</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="29" t="s">
@@ -4262,7 +4272,7 @@
       </c>
       <c r="I57" s="31"/>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="29" t="s">
         <v>82</v>
       </c>
@@ -4270,7 +4280,7 @@
         <v>231</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="29" t="s">
@@ -4287,7 +4297,7 @@
       </c>
       <c r="I58" s="31"/>
     </row>
-    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="29" t="s">
         <v>83</v>
       </c>
@@ -4295,7 +4305,7 @@
         <v>231</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29" t="s">
@@ -4312,7 +4322,7 @@
       </c>
       <c r="I59" s="31"/>
     </row>
-    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="29" t="s">
         <v>84</v>
       </c>
@@ -4320,7 +4330,7 @@
         <v>232</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="29" t="s">
@@ -4337,7 +4347,7 @@
       </c>
       <c r="I60" s="31"/>
     </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="29" t="s">
         <v>85</v>
       </c>
@@ -4345,7 +4355,7 @@
         <v>233</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D61" s="29"/>
       <c r="E61" s="29" t="s">
@@ -4362,7 +4372,7 @@
       </c>
       <c r="I61" s="31"/>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="29" t="s">
         <v>86</v>
       </c>
@@ -4370,7 +4380,7 @@
         <v>233</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29" t="s">
@@ -4387,7 +4397,7 @@
       </c>
       <c r="I62" s="31"/>
     </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="29" t="s">
         <v>87</v>
       </c>
@@ -4395,7 +4405,7 @@
         <v>233</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29" t="s">
@@ -4412,7 +4422,7 @@
       </c>
       <c r="I63" s="31"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="29" t="s">
         <v>88</v>
       </c>
@@ -4420,7 +4430,7 @@
         <v>233</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -4437,7 +4447,7 @@
       </c>
       <c r="I64" s="31"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="29" t="s">
         <v>89</v>
       </c>
@@ -4445,7 +4455,7 @@
         <v>233</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29" t="s">
@@ -4462,7 +4472,7 @@
       </c>
       <c r="I65" s="31"/>
     </row>
-    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="29" t="s">
         <v>90</v>
       </c>
@@ -4470,7 +4480,7 @@
         <v>233</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29" t="s">
@@ -4487,7 +4497,7 @@
       </c>
       <c r="I66" s="31"/>
     </row>
-    <row r="67" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" s="29" t="s">
         <v>91</v>
       </c>
@@ -4495,7 +4505,7 @@
         <v>233</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29" t="s">
@@ -4512,7 +4522,7 @@
       </c>
       <c r="I67" s="31"/>
     </row>
-    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="29" t="s">
         <v>92</v>
       </c>
@@ -4520,7 +4530,7 @@
         <v>234</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -4537,7 +4547,7 @@
       </c>
       <c r="I68" s="31"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="29" t="s">
         <v>93</v>
       </c>
@@ -4545,7 +4555,7 @@
         <v>234</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -4562,7 +4572,7 @@
       </c>
       <c r="I69" s="31"/>
     </row>
-    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="29" t="s">
         <v>94</v>
       </c>
@@ -4570,7 +4580,7 @@
         <v>234</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29" t="s">
@@ -4587,7 +4597,7 @@
       </c>
       <c r="I70" s="31"/>
     </row>
-    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="29" t="s">
         <v>95</v>
       </c>
@@ -4595,7 +4605,7 @@
         <v>234</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="29" t="s">
@@ -4612,7 +4622,7 @@
       </c>
       <c r="I71" s="31"/>
     </row>
-    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="29" t="s">
         <v>96</v>
       </c>
@@ -4620,7 +4630,7 @@
         <v>234</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D72" s="29"/>
       <c r="E72" s="29" t="s">
@@ -4637,7 +4647,7 @@
       </c>
       <c r="I72" s="31"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="29" t="s">
         <v>97</v>
       </c>
@@ -4645,7 +4655,7 @@
         <v>32</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29" t="s">
@@ -4662,7 +4672,7 @@
       </c>
       <c r="I73" s="31"/>
     </row>
-    <row r="74" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A74" s="29" t="s">
         <v>98</v>
       </c>
@@ -4670,7 +4680,7 @@
         <v>32</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29" t="s">
@@ -4687,7 +4697,7 @@
       </c>
       <c r="I74" s="31"/>
     </row>
-    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="29" t="s">
         <v>99</v>
       </c>
@@ -4695,7 +4705,7 @@
         <v>32</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="D75" s="29"/>
       <c r="E75" s="29" t="s">
@@ -4712,7 +4722,7 @@
       </c>
       <c r="I75" s="31"/>
     </row>
-    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="29" t="s">
         <v>100</v>
       </c>
@@ -4720,7 +4730,7 @@
         <v>235</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="29" t="s">
@@ -4737,7 +4747,7 @@
       </c>
       <c r="I76" s="31"/>
     </row>
-    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="29" t="s">
         <v>101</v>
       </c>
@@ -4745,7 +4755,7 @@
         <v>235</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D77" s="29"/>
       <c r="E77" s="29" t="s">
@@ -4762,7 +4772,7 @@
       </c>
       <c r="I77" s="31"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="29" t="s">
         <v>102</v>
       </c>
@@ -4770,7 +4780,7 @@
         <v>235</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D78" s="29"/>
       <c r="E78" s="29" t="s">
@@ -4787,7 +4797,7 @@
       </c>
       <c r="I78" s="31"/>
     </row>
-    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="29" t="s">
         <v>103</v>
       </c>
@@ -4795,7 +4805,7 @@
         <v>235</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D79" s="29"/>
       <c r="E79" s="29" t="s">
@@ -4812,7 +4822,7 @@
       </c>
       <c r="I79" s="31"/>
     </row>
-    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="29" t="s">
         <v>104</v>
       </c>
@@ -4820,7 +4830,7 @@
         <v>235</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D80" s="29"/>
       <c r="E80" s="29" t="s">
@@ -4837,7 +4847,7 @@
       </c>
       <c r="I80" s="31"/>
     </row>
-    <row r="81" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A81" s="29" t="s">
         <v>105</v>
       </c>
@@ -4845,7 +4855,7 @@
         <v>235</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D81" s="29"/>
       <c r="E81" s="29" t="s">
@@ -4861,10 +4871,10 @@
         <v>17</v>
       </c>
       <c r="I81" s="31" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="29" t="s">
         <v>106</v>
       </c>
@@ -4872,10 +4882,10 @@
         <v>235</v>
       </c>
       <c r="C82" s="31" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="E82" s="29" t="s">
         <v>19</v>
@@ -4891,7 +4901,7 @@
       </c>
       <c r="I82" s="31"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="29" t="s">
         <v>107</v>
       </c>
@@ -4899,10 +4909,10 @@
         <v>235</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="E83" s="29" t="s">
         <v>19</v>
@@ -4918,7 +4928,7 @@
       </c>
       <c r="I83" s="31"/>
     </row>
-    <row r="84" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" s="29" t="s">
         <v>108</v>
       </c>
@@ -4926,10 +4936,10 @@
         <v>235</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="E84" s="29" t="s">
         <v>19</v>
@@ -4945,7 +4955,7 @@
       </c>
       <c r="I84" s="31"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="29" t="s">
         <v>109</v>
       </c>
@@ -4953,10 +4963,10 @@
         <v>235</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="E85" s="29" t="s">
         <v>19</v>
@@ -4972,7 +4982,7 @@
       </c>
       <c r="I85" s="31"/>
     </row>
-    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="29" t="s">
         <v>110</v>
       </c>
@@ -4980,10 +4990,10 @@
         <v>235</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="E86" s="29" t="s">
         <v>19</v>
@@ -4999,7 +5009,7 @@
       </c>
       <c r="I86" s="31"/>
     </row>
-    <row r="87" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A87" s="29" t="s">
         <v>111</v>
       </c>
@@ -5007,7 +5017,7 @@
         <v>235</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="29" t="s">
@@ -5024,15 +5034,15 @@
       </c>
       <c r="I87" s="31"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="22" t="s">
-        <v>449</v>
+        <v>483</v>
       </c>
       <c r="B88" s="30" t="s">
         <v>235</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="29" t="s">
@@ -5049,7 +5059,7 @@
       </c>
       <c r="I88" s="31"/>
     </row>
-    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="22" t="s">
         <v>112</v>
       </c>
@@ -5057,7 +5067,7 @@
         <v>235</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29" t="s">
@@ -5074,15 +5084,15 @@
       </c>
       <c r="I89" s="31"/>
     </row>
-    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="22" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B90" s="30" t="s">
         <v>235</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="29" t="s">
@@ -5099,7 +5109,7 @@
       </c>
       <c r="I90" s="31"/>
     </row>
-    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="29" t="s">
         <v>113</v>
       </c>
@@ -5107,7 +5117,7 @@
         <v>235</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29" t="s">
@@ -5124,7 +5134,7 @@
       </c>
       <c r="I91" s="31"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="29" t="s">
         <v>114</v>
       </c>
@@ -5132,7 +5142,7 @@
         <v>235</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="29" t="s">
@@ -5149,7 +5159,7 @@
       </c>
       <c r="I92" s="31"/>
     </row>
-    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="29" t="s">
         <v>115</v>
       </c>
@@ -5157,7 +5167,7 @@
         <v>235</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="29" t="s">
@@ -5174,7 +5184,7 @@
       </c>
       <c r="I93" s="31"/>
     </row>
-    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="29" t="s">
         <v>116</v>
       </c>
@@ -5182,7 +5192,7 @@
         <v>236</v>
       </c>
       <c r="C94" s="31" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D94" s="29"/>
       <c r="E94" s="29" t="s">
@@ -5199,7 +5209,7 @@
       </c>
       <c r="I94" s="31"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="29" t="s">
         <v>117</v>
       </c>
@@ -5207,7 +5217,7 @@
         <v>236</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D95" s="29"/>
       <c r="E95" s="29" t="s">
@@ -5224,7 +5234,7 @@
       </c>
       <c r="I95" s="31"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="29" t="s">
         <v>118</v>
       </c>
@@ -5232,7 +5242,7 @@
         <v>237</v>
       </c>
       <c r="C96" s="31" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D96" s="29"/>
       <c r="E96" s="29" t="s">
@@ -5249,7 +5259,7 @@
       </c>
       <c r="I96" s="31"/>
     </row>
-    <row r="97" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="232" x14ac:dyDescent="0.35">
       <c r="A97" s="29" t="s">
         <v>119</v>
       </c>
@@ -5257,7 +5267,7 @@
         <v>237</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D97" s="29"/>
       <c r="E97" s="29" t="s">
@@ -5274,7 +5284,7 @@
       </c>
       <c r="I97" s="31"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="29" t="s">
         <v>120</v>
       </c>
@@ -5282,7 +5292,7 @@
         <v>237</v>
       </c>
       <c r="C98" s="31" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D98" s="29"/>
       <c r="E98" s="29" t="s">
@@ -5299,7 +5309,7 @@
       </c>
       <c r="I98" s="31"/>
     </row>
-    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A99" s="29" t="s">
         <v>121</v>
       </c>
@@ -5307,7 +5317,7 @@
         <v>237</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D99" s="29"/>
       <c r="E99" s="29" t="s">
@@ -5324,7 +5334,7 @@
       </c>
       <c r="I99" s="31"/>
     </row>
-    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="29" t="s">
         <v>122</v>
       </c>
@@ -5332,10 +5342,10 @@
         <v>237</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="E100" s="29" t="s">
         <v>19</v>
@@ -5351,7 +5361,7 @@
       </c>
       <c r="I100" s="31"/>
     </row>
-    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="29" t="s">
         <v>123</v>
       </c>
@@ -5359,10 +5369,10 @@
         <v>237</v>
       </c>
       <c r="C101" s="31" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="E101" s="29" t="s">
         <v>19</v>
@@ -5378,7 +5388,7 @@
       </c>
       <c r="I101" s="31"/>
     </row>
-    <row r="102" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="29" t="s">
         <v>124</v>
       </c>
@@ -5386,7 +5396,7 @@
         <v>237</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="29" t="s">
@@ -5403,7 +5413,7 @@
       </c>
       <c r="I102" s="31"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="29" t="s">
         <v>125</v>
       </c>
@@ -5411,7 +5421,7 @@
         <v>237</v>
       </c>
       <c r="C103" s="31" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D103" s="29"/>
       <c r="E103" s="29" t="s">
@@ -5428,7 +5438,7 @@
       </c>
       <c r="I103" s="31"/>
     </row>
-    <row r="104" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A104" s="22" t="s">
         <v>126</v>
       </c>
@@ -5436,7 +5446,7 @@
         <v>237</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29" t="s">
@@ -5453,18 +5463,18 @@
       </c>
       <c r="I104" s="31"/>
     </row>
-    <row r="105" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A105" s="22" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="B105" s="30" t="s">
         <v>237</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="D105" s="22" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="E105" s="29" t="s">
         <v>19</v>
@@ -5480,18 +5490,18 @@
       </c>
       <c r="I105" s="31"/>
     </row>
-    <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A106" s="22" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="B106" s="30" t="s">
         <v>237</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="D106" s="22" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="E106" s="29" t="s">
         <v>19</v>
@@ -5507,7 +5517,7 @@
       </c>
       <c r="I106" s="31"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="29" t="s">
         <v>127</v>
       </c>
@@ -5515,7 +5525,7 @@
         <v>237</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="29" t="s">
@@ -5532,7 +5542,7 @@
       </c>
       <c r="I107" s="31"/>
     </row>
-    <row r="108" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A108" s="29" t="s">
         <v>128</v>
       </c>
@@ -5540,7 +5550,7 @@
         <v>237</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="29" t="s">
@@ -5556,10 +5566,10 @@
         <v>17</v>
       </c>
       <c r="I108" s="31" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="29" t="s">
         <v>129</v>
       </c>
@@ -5567,10 +5577,10 @@
         <v>237</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D109" s="29" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="E109" s="29" t="s">
         <v>19</v>
@@ -5586,7 +5596,7 @@
       </c>
       <c r="I109" s="31"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="29" t="s">
         <v>130</v>
       </c>
@@ -5594,10 +5604,10 @@
         <v>237</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D110" s="29" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="E110" s="29" t="s">
         <v>19</v>
@@ -5613,7 +5623,7 @@
       </c>
       <c r="I110" s="31"/>
     </row>
-    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="29" t="s">
         <v>131</v>
       </c>
@@ -5621,10 +5631,10 @@
         <v>237</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D111" s="29" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="E111" s="29" t="s">
         <v>19</v>
@@ -5640,7 +5650,7 @@
       </c>
       <c r="I111" s="31"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="29" t="s">
         <v>132</v>
       </c>
@@ -5648,7 +5658,7 @@
         <v>237</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="29" t="s">
@@ -5665,7 +5675,7 @@
       </c>
       <c r="I112" s="31"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="29" t="s">
         <v>133</v>
       </c>
@@ -5673,7 +5683,7 @@
         <v>237</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D113" s="29"/>
       <c r="E113" s="29" t="s">
@@ -5690,7 +5700,7 @@
       </c>
       <c r="I113" s="31"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="29" t="s">
         <v>134</v>
       </c>
@@ -5698,7 +5708,7 @@
         <v>237</v>
       </c>
       <c r="C114" s="31" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="29" t="s">
@@ -5715,7 +5725,7 @@
       </c>
       <c r="I114" s="31"/>
     </row>
-    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="29" t="s">
         <v>135</v>
       </c>
@@ -5723,7 +5733,7 @@
         <v>237</v>
       </c>
       <c r="C115" s="31" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -5740,7 +5750,7 @@
       </c>
       <c r="I115" s="31"/>
     </row>
-    <row r="116" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="29" t="s">
         <v>136</v>
       </c>
@@ -5748,7 +5758,7 @@
         <v>237</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="29" t="s">
@@ -5764,10 +5774,10 @@
         <v>17</v>
       </c>
       <c r="I116" s="31" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="29" t="s">
         <v>137</v>
       </c>
@@ -5775,7 +5785,7 @@
         <v>237</v>
       </c>
       <c r="C117" s="31" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="29" t="s">
@@ -5792,7 +5802,7 @@
       </c>
       <c r="I117" s="31"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="29" t="s">
         <v>138</v>
       </c>
@@ -5800,7 +5810,7 @@
         <v>237</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="29" t="s">
@@ -5817,7 +5827,7 @@
       </c>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="29" t="s">
         <v>139</v>
       </c>
@@ -5825,7 +5835,7 @@
         <v>237</v>
       </c>
       <c r="C119" s="31" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="29" t="s">
@@ -5842,7 +5852,7 @@
       </c>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="29" t="s">
         <v>140</v>
       </c>
@@ -5850,7 +5860,7 @@
         <v>237</v>
       </c>
       <c r="C120" s="31" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D120" s="29"/>
       <c r="E120" s="29" t="s">
@@ -5867,7 +5877,7 @@
       </c>
       <c r="I120" s="31"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="29" t="s">
         <v>141</v>
       </c>
@@ -5875,7 +5885,7 @@
         <v>237</v>
       </c>
       <c r="C121" s="31" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="29" t="s">
@@ -5892,7 +5902,7 @@
       </c>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="29" t="s">
         <v>142</v>
       </c>
@@ -5900,7 +5910,7 @@
         <v>237</v>
       </c>
       <c r="C122" s="20" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="29" t="s">
@@ -5917,15 +5927,15 @@
       </c>
       <c r="I122" s="31"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="22" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="B123" s="30" t="s">
         <v>237</v>
       </c>
       <c r="C123" s="20" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -5942,7 +5952,7 @@
       </c>
       <c r="I123" s="31"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="29" t="s">
         <v>143</v>
       </c>
@@ -5950,7 +5960,7 @@
         <v>237</v>
       </c>
       <c r="C124" s="31" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="29" t="s">
@@ -5967,7 +5977,7 @@
       </c>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A125" s="29" t="s">
         <v>144</v>
       </c>
@@ -5975,7 +5985,7 @@
         <v>237</v>
       </c>
       <c r="C125" s="31" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29" t="s">
@@ -5991,10 +6001,10 @@
         <v>17</v>
       </c>
       <c r="I125" s="31" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A126" s="29" t="s">
         <v>145</v>
       </c>
@@ -6002,10 +6012,10 @@
         <v>237</v>
       </c>
       <c r="C126" s="31" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D126" s="29" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="E126" s="29" t="s">
         <v>19</v>
@@ -6021,7 +6031,7 @@
       </c>
       <c r="I126" s="31"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A127" s="29" t="s">
         <v>146</v>
       </c>
@@ -6029,10 +6039,10 @@
         <v>237</v>
       </c>
       <c r="C127" s="31" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D127" s="29" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="E127" s="29" t="s">
         <v>19</v>
@@ -6048,7 +6058,7 @@
       </c>
       <c r="I127" s="31"/>
     </row>
-    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="29" t="s">
         <v>147</v>
       </c>
@@ -6056,10 +6066,10 @@
         <v>237</v>
       </c>
       <c r="C128" s="31" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="D128" s="29" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="E128" s="29" t="s">
         <v>19</v>
@@ -6075,7 +6085,7 @@
       </c>
       <c r="I128" s="31"/>
     </row>
-    <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A129" s="29" t="s">
         <v>148</v>
       </c>
@@ -6083,7 +6093,7 @@
         <v>237</v>
       </c>
       <c r="C129" s="31" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="29" t="s">
@@ -6100,7 +6110,7 @@
       </c>
       <c r="I129" s="31"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="29" t="s">
         <v>149</v>
       </c>
@@ -6108,7 +6118,7 @@
         <v>237</v>
       </c>
       <c r="C130" s="31" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="29" t="s">
@@ -6125,7 +6135,7 @@
       </c>
       <c r="I130" s="31"/>
     </row>
-    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A131" s="29" t="s">
         <v>150</v>
       </c>
@@ -6133,7 +6143,7 @@
         <v>237</v>
       </c>
       <c r="C131" s="31" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -6149,10 +6159,10 @@
         <v>17</v>
       </c>
       <c r="I131" s="31" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="29" t="s">
         <v>151</v>
       </c>
@@ -6160,10 +6170,10 @@
         <v>237</v>
       </c>
       <c r="C132" s="31" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D132" s="29" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="E132" s="29" t="s">
         <v>19</v>
@@ -6179,7 +6189,7 @@
       </c>
       <c r="I132" s="31"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="29" t="s">
         <v>152</v>
       </c>
@@ -6187,10 +6197,10 @@
         <v>237</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="E133" s="29" t="s">
         <v>19</v>
@@ -6206,7 +6216,7 @@
       </c>
       <c r="I133" s="31"/>
     </row>
-    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A134" s="29" t="s">
         <v>153</v>
       </c>
@@ -6214,10 +6224,10 @@
         <v>237</v>
       </c>
       <c r="C134" s="31" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="D134" s="29" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="E134" s="29" t="s">
         <v>19</v>
@@ -6233,7 +6243,7 @@
       </c>
       <c r="I134" s="31"/>
     </row>
-    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A135" s="29" t="s">
         <v>154</v>
       </c>
@@ -6241,7 +6251,7 @@
         <v>237</v>
       </c>
       <c r="C135" s="31" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="29" t="s">
@@ -6258,7 +6268,7 @@
       </c>
       <c r="I135" s="31"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="29" t="s">
         <v>155</v>
       </c>
@@ -6266,7 +6276,7 @@
         <v>237</v>
       </c>
       <c r="C136" s="31" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="29" t="s">
@@ -6283,7 +6293,7 @@
       </c>
       <c r="I136" s="31"/>
     </row>
-    <row r="137" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A137" s="29" t="s">
         <v>156</v>
       </c>
@@ -6291,7 +6301,7 @@
         <v>237</v>
       </c>
       <c r="C137" s="31" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="29" t="s">
@@ -6307,10 +6317,10 @@
         <v>17</v>
       </c>
       <c r="I137" s="31" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="29" t="s">
         <v>157</v>
       </c>
@@ -6318,10 +6328,10 @@
         <v>237</v>
       </c>
       <c r="C138" s="31" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D138" s="29" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="E138" s="29" t="s">
         <v>19</v>
@@ -6337,7 +6347,7 @@
       </c>
       <c r="I138" s="31"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="29" t="s">
         <v>158</v>
       </c>
@@ -6345,10 +6355,10 @@
         <v>237</v>
       </c>
       <c r="C139" s="31" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D139" s="29" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="E139" s="29" t="s">
         <v>19</v>
@@ -6364,7 +6374,7 @@
       </c>
       <c r="I139" s="31"/>
     </row>
-    <row r="140" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A140" s="29" t="s">
         <v>159</v>
       </c>
@@ -6372,10 +6382,10 @@
         <v>237</v>
       </c>
       <c r="C140" s="31" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="D140" s="29" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="E140" s="29" t="s">
         <v>19</v>
@@ -6391,7 +6401,7 @@
       </c>
       <c r="I140" s="31"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" s="29" t="s">
         <v>160</v>
       </c>
@@ -6399,7 +6409,7 @@
         <v>237</v>
       </c>
       <c r="C141" s="31" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="29" t="s">
@@ -6416,7 +6426,7 @@
       </c>
       <c r="I141" s="31"/>
     </row>
-    <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A142" s="29" t="s">
         <v>161</v>
       </c>
@@ -6424,7 +6434,7 @@
         <v>237</v>
       </c>
       <c r="C142" s="31" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="29" t="s">
@@ -6441,7 +6451,7 @@
       </c>
       <c r="I142" s="31"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" s="29" t="s">
         <v>162</v>
       </c>
@@ -6449,7 +6459,7 @@
         <v>237</v>
       </c>
       <c r="C143" s="31" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -6466,7 +6476,7 @@
       </c>
       <c r="I143" s="31"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" s="29" t="s">
         <v>163</v>
       </c>
@@ -6474,7 +6484,7 @@
         <v>237</v>
       </c>
       <c r="C144" s="31" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="29" t="s">
@@ -6491,7 +6501,7 @@
       </c>
       <c r="I144" s="31"/>
     </row>
-    <row r="145" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A145" s="29" t="s">
         <v>164</v>
       </c>
@@ -6499,7 +6509,7 @@
         <v>237</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D145" s="29"/>
       <c r="E145" s="29" t="s">
@@ -6515,10 +6525,10 @@
         <v>17</v>
       </c>
       <c r="I145" s="31" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" s="29" t="s">
         <v>165</v>
       </c>
@@ -6526,10 +6536,10 @@
         <v>237</v>
       </c>
       <c r="C146" s="31" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="E146" s="29" t="s">
         <v>19</v>
@@ -6545,7 +6555,7 @@
       </c>
       <c r="I146" s="31"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" s="29" t="s">
         <v>166</v>
       </c>
@@ -6553,10 +6563,10 @@
         <v>237</v>
       </c>
       <c r="C147" s="31" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D147" s="29" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="E147" s="29" t="s">
         <v>19</v>
@@ -6572,7 +6582,7 @@
       </c>
       <c r="I147" s="31"/>
     </row>
-    <row r="148" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A148" s="29" t="s">
         <v>167</v>
       </c>
@@ -6580,10 +6590,10 @@
         <v>237</v>
       </c>
       <c r="C148" s="31" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="E148" s="29" t="s">
         <v>19</v>
@@ -6599,7 +6609,7 @@
       </c>
       <c r="I148" s="31"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" s="29" t="s">
         <v>168</v>
       </c>
@@ -6607,7 +6617,7 @@
         <v>237</v>
       </c>
       <c r="C149" s="31" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="29" t="s">
@@ -6624,7 +6634,7 @@
       </c>
       <c r="I149" s="31"/>
     </row>
-    <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="29" t="s">
         <v>169</v>
       </c>
@@ -6632,7 +6642,7 @@
         <v>238</v>
       </c>
       <c r="C150" s="31" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="29" t="s">
@@ -6649,7 +6659,7 @@
       </c>
       <c r="I150" s="31"/>
     </row>
-    <row r="151" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A151" s="29" t="s">
         <v>170</v>
       </c>
@@ -6657,7 +6667,7 @@
         <v>238</v>
       </c>
       <c r="C151" s="31" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="29" t="s">
@@ -6674,7 +6684,7 @@
       </c>
       <c r="I151" s="31"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" s="22" t="s">
         <v>171</v>
       </c>
@@ -6682,7 +6692,7 @@
         <v>238</v>
       </c>
       <c r="C152" s="20" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="29" t="s">
@@ -6699,15 +6709,15 @@
       </c>
       <c r="I152" s="31"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" s="22" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="B153" s="30" t="s">
         <v>238</v>
       </c>
       <c r="C153" s="20" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
@@ -6724,7 +6734,7 @@
       </c>
       <c r="I153" s="31"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" s="29" t="s">
         <v>172</v>
       </c>
@@ -6732,7 +6742,7 @@
         <v>33</v>
       </c>
       <c r="C154" s="31" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="29" t="s">
@@ -6749,7 +6759,7 @@
       </c>
       <c r="I154" s="31"/>
     </row>
-    <row r="155" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A155" s="29" t="s">
         <v>173</v>
       </c>
@@ -6757,7 +6767,7 @@
         <v>33</v>
       </c>
       <c r="C155" s="31" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="29" t="s">
@@ -6774,7 +6784,7 @@
       </c>
       <c r="I155" s="31"/>
     </row>
-    <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A156" s="29" t="s">
         <v>174</v>
       </c>
@@ -6782,7 +6792,7 @@
         <v>33</v>
       </c>
       <c r="C156" s="31" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="29" t="s">
@@ -6799,7 +6809,7 @@
       </c>
       <c r="I156" s="31"/>
     </row>
-    <row r="157" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A157" s="29" t="s">
         <v>175</v>
       </c>
@@ -6807,7 +6817,7 @@
         <v>33</v>
       </c>
       <c r="C157" s="31" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="D157" s="29"/>
       <c r="E157" s="29" t="s">
@@ -6824,7 +6834,7 @@
       </c>
       <c r="I157" s="31"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" s="29" t="s">
         <v>176</v>
       </c>
@@ -6832,7 +6842,7 @@
         <v>239</v>
       </c>
       <c r="C158" s="31" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D158" s="29"/>
       <c r="E158" s="29" t="s">
@@ -6849,7 +6859,7 @@
       </c>
       <c r="I158" s="31"/>
     </row>
-    <row r="159" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A159" s="29" t="s">
         <v>177</v>
       </c>
@@ -6857,7 +6867,7 @@
         <v>239</v>
       </c>
       <c r="C159" s="31" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="D159" s="29"/>
       <c r="E159" s="29" t="s">
@@ -6874,7 +6884,7 @@
       </c>
       <c r="I159" s="31"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" s="29" t="s">
         <v>178</v>
       </c>
@@ -6882,7 +6892,7 @@
         <v>239</v>
       </c>
       <c r="C160" s="31" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="D160" s="29"/>
       <c r="E160" s="29" t="s">
@@ -6899,7 +6909,7 @@
       </c>
       <c r="I160" s="31"/>
     </row>
-    <row r="161" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
         <v>179</v>
       </c>
@@ -6907,7 +6917,7 @@
         <v>239</v>
       </c>
       <c r="C161" s="31" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="D161" s="29"/>
       <c r="E161" s="29" t="s">
@@ -6924,7 +6934,7 @@
       </c>
       <c r="I161" s="31"/>
     </row>
-    <row r="162" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
         <v>180</v>
       </c>
@@ -6932,7 +6942,7 @@
         <v>239</v>
       </c>
       <c r="C162" s="31" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="D162" s="29"/>
       <c r="E162" s="29" t="s">
@@ -6949,7 +6959,7 @@
       </c>
       <c r="I162" s="31"/>
     </row>
-    <row r="163" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
         <v>181</v>
       </c>
@@ -6957,7 +6967,7 @@
         <v>239</v>
       </c>
       <c r="C163" s="31" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="D163" s="29"/>
       <c r="E163" s="29" t="s">
@@ -6974,7 +6984,7 @@
       </c>
       <c r="I163" s="31"/>
     </row>
-    <row r="164" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
         <v>182</v>
       </c>
@@ -6982,7 +6992,7 @@
         <v>239</v>
       </c>
       <c r="C164" s="31" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="29" t="s">
@@ -6999,7 +7009,7 @@
       </c>
       <c r="I164" s="31"/>
     </row>
-    <row r="165" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A165" s="29" t="s">
         <v>183</v>
       </c>
@@ -7007,7 +7017,7 @@
         <v>240</v>
       </c>
       <c r="C165" s="31" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -7024,7 +7034,7 @@
       </c>
       <c r="I165" s="31"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" s="29" t="s">
         <v>184</v>
       </c>
@@ -7032,7 +7042,7 @@
         <v>240</v>
       </c>
       <c r="C166" s="31" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="D166" s="29"/>
       <c r="E166" s="29" t="s">
@@ -7049,7 +7059,7 @@
       </c>
       <c r="I166" s="31"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" s="29" t="s">
         <v>185</v>
       </c>
@@ -7057,7 +7067,7 @@
         <v>241</v>
       </c>
       <c r="C167" s="31" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="D167" s="29"/>
       <c r="E167" s="29" t="s">
@@ -7074,7 +7084,7 @@
       </c>
       <c r="I167" s="31"/>
     </row>
-    <row r="168" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A168" s="29" t="s">
         <v>186</v>
       </c>
@@ -7082,7 +7092,7 @@
         <v>241</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="D168" s="29"/>
       <c r="E168" s="29" t="s">
@@ -7099,7 +7109,7 @@
       </c>
       <c r="I168" s="31"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" s="29" t="s">
         <v>187</v>
       </c>
@@ -7107,7 +7117,7 @@
         <v>241</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D169" s="29"/>
       <c r="E169" s="29" t="s">
@@ -7124,7 +7134,7 @@
       </c>
       <c r="I169" s="31"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A170" s="29" t="s">
         <v>188</v>
       </c>
@@ -7132,7 +7142,7 @@
         <v>242</v>
       </c>
       <c r="C170" s="31" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="D170" s="29"/>
       <c r="E170" s="29" t="s">
@@ -7149,7 +7159,7 @@
       </c>
       <c r="I170" s="31"/>
     </row>
-    <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="29" t="s">
         <v>189</v>
       </c>
@@ -7157,7 +7167,7 @@
         <v>242</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="D171" s="29"/>
       <c r="E171" s="29" t="s">
@@ -7174,7 +7184,7 @@
       </c>
       <c r="I171" s="31"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A172" s="29" t="s">
         <v>190</v>
       </c>
@@ -7182,7 +7192,7 @@
         <v>243</v>
       </c>
       <c r="C172" s="31" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="D172" s="29"/>
       <c r="E172" s="29" t="s">
@@ -7199,7 +7209,7 @@
       </c>
       <c r="I172" s="31"/>
     </row>
-    <row r="173" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A173" s="29" t="s">
         <v>191</v>
       </c>
@@ -7207,7 +7217,7 @@
         <v>243</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="29" t="s">
@@ -7224,7 +7234,7 @@
       </c>
       <c r="I173" s="31"/>
     </row>
-    <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="29" t="s">
         <v>192</v>
       </c>
@@ -7232,7 +7242,7 @@
         <v>243</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D174" s="29"/>
       <c r="E174" s="29" t="s">
@@ -7249,7 +7259,7 @@
       </c>
       <c r="I174" s="31"/>
     </row>
-    <row r="175" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="29" t="s">
         <v>193</v>
       </c>
@@ -7257,7 +7267,7 @@
         <v>244</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="29" t="s">
@@ -7274,7 +7284,7 @@
       </c>
       <c r="I175" s="31"/>
     </row>
-    <row r="176" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A176" s="29" t="s">
         <v>194</v>
       </c>
@@ -7282,7 +7292,7 @@
         <v>244</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D176" s="29"/>
       <c r="E176" s="29" t="s">
@@ -7299,7 +7309,7 @@
       </c>
       <c r="I176" s="31"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" s="29" t="s">
         <v>195</v>
       </c>
@@ -7307,7 +7317,7 @@
         <v>244</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="D177" s="29"/>
       <c r="E177" s="29" t="s">
@@ -7324,7 +7334,7 @@
       </c>
       <c r="I177" s="31"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="29" t="s">
         <v>196</v>
       </c>
@@ -7332,7 +7342,7 @@
         <v>245</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="D178" s="29"/>
       <c r="E178" s="29" t="s">
@@ -7349,7 +7359,7 @@
       </c>
       <c r="I178" s="31"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" s="29" t="s">
         <v>197</v>
       </c>
@@ -7357,7 +7367,7 @@
         <v>245</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="D179" s="29"/>
       <c r="E179" s="29" t="s">
@@ -7374,7 +7384,7 @@
       </c>
       <c r="I179" s="31"/>
     </row>
-    <row r="180" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="29" t="s">
         <v>198</v>
       </c>
@@ -7382,7 +7392,7 @@
         <v>246</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="D180" s="29"/>
       <c r="E180" s="29" t="s">
@@ -7399,7 +7409,7 @@
       </c>
       <c r="I180" s="31"/>
     </row>
-    <row r="181" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A181" s="29" t="s">
         <v>199</v>
       </c>
@@ -7407,7 +7417,7 @@
         <v>246</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="D181" s="29"/>
       <c r="E181" s="29" t="s">
@@ -7424,7 +7434,7 @@
       </c>
       <c r="I181" s="31"/>
     </row>
-    <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" s="29" t="s">
         <v>200</v>
       </c>
@@ -7432,7 +7442,7 @@
         <v>247</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="D182" s="29"/>
       <c r="E182" s="29" t="s">
@@ -7449,7 +7459,7 @@
       </c>
       <c r="I182" s="31"/>
     </row>
-    <row r="183" spans="1:9" ht="300" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" ht="290" x14ac:dyDescent="0.35">
       <c r="A183" s="29" t="s">
         <v>201</v>
       </c>
@@ -7457,7 +7467,7 @@
         <v>247</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="D183" s="29"/>
       <c r="E183" s="29" t="s">
@@ -7474,7 +7484,7 @@
       </c>
       <c r="I183" s="31"/>
     </row>
-    <row r="184" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A184" s="22" t="s">
         <v>202</v>
       </c>
@@ -7482,7 +7492,7 @@
         <v>247</v>
       </c>
       <c r="C184" s="20" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="29" t="s">
@@ -7499,15 +7509,15 @@
       </c>
       <c r="I184" s="31"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" s="22" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="B185" s="24" t="s">
         <v>247</v>
       </c>
       <c r="C185" s="20" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="D185" s="29"/>
       <c r="E185" s="29" t="s">
@@ -7524,15 +7534,15 @@
       </c>
       <c r="I185" s="31"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A186" s="22" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="B186" s="24" t="s">
         <v>247</v>
       </c>
       <c r="C186" s="20" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="29" t="s">
@@ -7549,7 +7559,7 @@
       </c>
       <c r="I186" s="31"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="29" t="s">
         <v>203</v>
       </c>
@@ -7557,7 +7567,7 @@
         <v>248</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="29" t="s">
@@ -7574,7 +7584,7 @@
       </c>
       <c r="I187" s="31"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" s="29" t="s">
         <v>204</v>
       </c>
@@ -7582,7 +7592,7 @@
         <v>248</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="29" t="s">
@@ -7599,7 +7609,7 @@
       </c>
       <c r="I188" s="31"/>
     </row>
-    <row r="189" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A189" s="29" t="s">
         <v>205</v>
       </c>
@@ -7607,7 +7617,7 @@
         <v>248</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="D189" s="29"/>
       <c r="E189" s="29" t="s">
@@ -7624,7 +7634,7 @@
       </c>
       <c r="I189" s="31"/>
     </row>
-    <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="29" t="s">
         <v>206</v>
       </c>
@@ -7632,7 +7642,7 @@
         <v>248</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="D190" s="29"/>
       <c r="E190" s="29" t="s">
@@ -7649,7 +7659,7 @@
       </c>
       <c r="I190" s="31"/>
     </row>
-    <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A191" s="29" t="s">
         <v>207</v>
       </c>
@@ -7657,7 +7667,7 @@
         <v>249</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="D191" s="29"/>
       <c r="E191" s="29" t="s">
@@ -7674,7 +7684,7 @@
       </c>
       <c r="I191" s="31"/>
     </row>
-    <row r="192" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A192" s="29" t="s">
         <v>208</v>
       </c>
@@ -7682,7 +7692,7 @@
         <v>249</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="D192" s="29"/>
       <c r="E192" s="29" t="s">
@@ -7699,7 +7709,7 @@
       </c>
       <c r="I192" s="31"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" s="29" t="s">
         <v>209</v>
       </c>
@@ -7707,7 +7717,7 @@
         <v>249</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="D193" s="29"/>
       <c r="E193" s="29" t="s">
@@ -7724,7 +7734,7 @@
       </c>
       <c r="I193" s="31"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A194" s="29" t="s">
         <v>210</v>
       </c>
@@ -7732,7 +7742,7 @@
         <v>250</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="29" t="s">
@@ -7749,7 +7759,7 @@
       </c>
       <c r="I194" s="31"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" s="29" t="s">
         <v>211</v>
       </c>
@@ -7757,7 +7767,7 @@
         <v>250</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="D195" s="29"/>
       <c r="E195" s="29" t="s">
@@ -7774,7 +7784,7 @@
       </c>
       <c r="I195" s="31"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" s="29" t="s">
         <v>212</v>
       </c>
@@ -7782,7 +7792,7 @@
         <v>251</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -7799,7 +7809,7 @@
       </c>
       <c r="I196" s="31"/>
     </row>
-    <row r="197" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A197" s="29" t="s">
         <v>213</v>
       </c>
@@ -7807,7 +7817,7 @@
         <v>251</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="D197" s="29"/>
       <c r="E197" s="29" t="s">
@@ -7824,7 +7834,7 @@
       </c>
       <c r="I197" s="31"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" s="22" t="s">
         <v>214</v>
       </c>
@@ -7832,7 +7842,7 @@
         <v>251</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -7849,15 +7859,15 @@
       </c>
       <c r="I198" s="31"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" s="22" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="B199" s="30" t="s">
         <v>251</v>
       </c>
       <c r="C199" s="20" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="D199" s="29"/>
       <c r="E199" s="29" t="s">
@@ -7874,7 +7884,7 @@
       </c>
       <c r="I199" s="31"/>
     </row>
-    <row r="200" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="29" t="s">
         <v>215</v>
       </c>
@@ -7882,7 +7892,7 @@
         <v>251</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="D200" s="29"/>
       <c r="E200" s="29" t="s">
@@ -7899,7 +7909,7 @@
       </c>
       <c r="I200" s="31"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A201" s="29" t="s">
         <v>216</v>
       </c>
@@ -7907,7 +7917,7 @@
         <v>252</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -7924,7 +7934,7 @@
       </c>
       <c r="I201" s="31"/>
     </row>
-    <row r="202" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A202" s="22" t="s">
         <v>217</v>
       </c>
@@ -7932,7 +7942,7 @@
         <v>252</v>
       </c>
       <c r="C202" s="31" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="D202" s="29"/>
       <c r="E202" s="29" t="s">
@@ -7949,15 +7959,15 @@
       </c>
       <c r="I202" s="31"/>
     </row>
-    <row r="203" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="22" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="B203" s="24" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="C203" s="20" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="D203" s="29"/>
       <c r="E203" s="29" t="s">
@@ -7974,15 +7984,15 @@
       </c>
       <c r="I203" s="31"/>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" s="22" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="B204" s="24" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="C204" s="20" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="D204" s="29"/>
       <c r="E204" s="29" t="s">
@@ -7999,15 +8009,15 @@
       </c>
       <c r="I204" s="31"/>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" s="22" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="B205" s="24" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="C205" s="20" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="D205" s="29"/>
       <c r="E205" s="29" t="s">
@@ -8024,15 +8034,15 @@
       </c>
       <c r="I205" s="31"/>
     </row>
-    <row r="206" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A206" s="22" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="B206" s="24" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="C206" s="20" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="D206" s="29"/>
       <c r="E206" s="29" t="s">
@@ -8049,7 +8059,7 @@
       </c>
       <c r="I206" s="31"/>
     </row>
-    <row r="207" spans="1:9" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:9" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A207" s="22" t="s">
         <v>45</v>
       </c>
@@ -8060,7 +8070,7 @@
         <v>256</v>
       </c>
       <c r="D207" s="22" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="E207" s="22" t="s">
         <v>22</v>
@@ -8075,10 +8085,10 @@
         <v>21</v>
       </c>
       <c r="I207" s="24" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A208" s="29" t="s">
         <v>218</v>
       </c>
@@ -8086,7 +8096,7 @@
         <v>253</v>
       </c>
       <c r="C208" s="31" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -8103,7 +8113,7 @@
       </c>
       <c r="I208" s="31"/>
     </row>
-    <row r="209" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A209" s="29" t="s">
         <v>219</v>
       </c>
@@ -8111,7 +8121,7 @@
         <v>253</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D209" s="29"/>
       <c r="E209" s="29" t="s">
@@ -8128,7 +8138,7 @@
       </c>
       <c r="I209" s="31"/>
     </row>
-    <row r="210" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A210" s="29" t="s">
         <v>220</v>
       </c>
@@ -8136,10 +8146,10 @@
         <v>253</v>
       </c>
       <c r="C210" s="20" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="D210" s="24" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="E210" s="29" t="s">
         <v>22</v>
@@ -8154,10 +8164,10 @@
         <v>20</v>
       </c>
       <c r="I210" s="31" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A211" s="29" t="s">
         <v>221</v>
       </c>
@@ -8165,7 +8175,7 @@
         <v>253</v>
       </c>
       <c r="C211" s="20" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="D211" s="29"/>
       <c r="E211" s="29" t="s">
@@ -8182,11 +8192,11 @@
       </c>
       <c r="I211" s="31"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" s="3"/>
       <c r="B212" s="10"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" s="3"/>
       <c r="B213" s="10"/>
     </row>
@@ -8237,20 +8247,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F211">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F211" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E211">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E211" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G211">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G211" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H211">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H211" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8270,6 +8280,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -8318,22 +8343,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8346,26 +8378,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-ADMINS: Fix failed cases on SharePoint 2019.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-ADMINS/MS-ADMINS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-ADMINS/MS-ADMINS_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F4DE3-1B8F-4C1A-B712-38733A681716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936192AC-EEBE-49B5-8D2B-770BEFB24E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$210</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="482">
   <si>
     <t>Req ID</t>
   </si>
@@ -717,15 +717,6 @@
     <t>MS-ADMINS_R71</t>
   </si>
   <si>
-    <t>MS-ADMINS_R3027</t>
-  </si>
-  <si>
-    <t>MS-ADMINS_R3038</t>
-  </si>
-  <si>
-    <t>MS-ADMINS_R3028</t>
-  </si>
-  <si>
     <t>MS-ADMINS_R2057</t>
   </si>
   <si>
@@ -1349,9 +1340,6 @@
   </si>
   <si>
     <t>[In CreateSite]If the length of the PortalUrl is 260 characters, the CreateSite operation will succeed.</t>
-  </si>
-  <si>
-    <t>[In CreateSite]If the length of the PortalUrl exceeds 260 characters, the CreateSite operation will succeed without exception, the exceeds characters are truncated.</t>
   </si>
   <si>
     <t>[In CreateSite]If [the PortalUrl] nothing is specified, no portal URL will be set in the database.</t>
@@ -1629,9 +1617,6 @@
     <t>Partially verified by derived requirements: MS-ADMINS_R3025, MS-ADMINS_R3013, MS-ADMINS_R3026.</t>
   </si>
   <si>
-    <t>Partially verified by derived requirements: MS-ADMINS_R3027, MS-ADMINS_R3038, MS-ADMINS_R3028.</t>
-  </si>
-  <si>
     <t>Partially verified by derived requirements: MS-ADMINS_R3029, MS-ADMINS_R3039, MS-ADMINS_R3030.</t>
   </si>
   <si>
@@ -1790,6 +1775,18 @@
   </si>
   <si>
     <t>MS-ADMINS_R18001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-ADMINS_R3027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Partially verified by derived requirements: MS-ADMINS_R3027, MS-ADMINS_R3038.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-ADMINS_R3038</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2066,6 +2063,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2090,26 +2102,55 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2448,50 +2489,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2621,34 +2618,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I211" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I211" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I210" tableType="xml" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" connectionId="1">
+  <autoFilter ref="A19:I210" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="24">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="23">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="19">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="18">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="17">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2657,12 +2654,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2990,7 +2987,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L213"/>
+  <dimension ref="A1:L212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3011,7 +3008,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -3021,7 +3018,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3035,10 +3032,10 @@
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F3" s="12">
         <v>43634</v>
@@ -3046,127 +3043,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -3179,12 +3176,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3197,12 +3194,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -3215,12 +3212,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -3233,60 +3230,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -3325,10 +3322,10 @@
         <v>43</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22" t="s">
@@ -3350,10 +3347,10 @@
         <v>44</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="s">
@@ -3369,7 +3366,7 @@
         <v>17</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.25">
@@ -3377,10 +3374,10 @@
         <v>46</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
@@ -3402,10 +3399,10 @@
         <v>47</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="s">
@@ -3427,10 +3424,10 @@
         <v>48</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="s">
@@ -3452,10 +3449,10 @@
         <v>49</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -3477,10 +3474,10 @@
         <v>50</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
@@ -3502,10 +3499,10 @@
         <v>51</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22" t="s">
@@ -3527,10 +3524,10 @@
         <v>52</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
@@ -3552,10 +3549,10 @@
         <v>53</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22" t="s">
@@ -3577,10 +3574,10 @@
         <v>54</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -3602,10 +3599,10 @@
         <v>55</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22" t="s">
@@ -3627,10 +3624,10 @@
         <v>56</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -3652,10 +3649,10 @@
         <v>57</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="29" t="s">
@@ -3677,10 +3674,10 @@
         <v>58</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29" t="s">
@@ -3702,10 +3699,10 @@
         <v>59</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29" t="s">
@@ -3727,10 +3724,10 @@
         <v>60</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29" t="s">
@@ -3752,10 +3749,10 @@
         <v>61</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
@@ -3777,10 +3774,10 @@
         <v>62</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29" t="s">
@@ -3802,10 +3799,10 @@
         <v>63</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29" t="s">
@@ -3827,10 +3824,10 @@
         <v>64</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29" t="s">
@@ -3852,10 +3849,10 @@
         <v>65</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29" t="s">
@@ -3880,7 +3877,7 @@
         <v>31</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29" t="s">
@@ -3905,7 +3902,7 @@
         <v>31</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -3930,7 +3927,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29" t="s">
@@ -3955,7 +3952,7 @@
         <v>31</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29" t="s">
@@ -3980,7 +3977,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29" t="s">
@@ -4002,10 +3999,10 @@
         <v>71</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29" t="s">
@@ -4027,10 +4024,10 @@
         <v>72</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29" t="s">
@@ -4052,10 +4049,10 @@
         <v>73</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29" t="s">
@@ -4077,10 +4074,10 @@
         <v>74</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="29" t="s">
@@ -4102,10 +4099,10 @@
         <v>75</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="29" t="s">
@@ -4127,10 +4124,10 @@
         <v>76</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D52" s="29"/>
       <c r="E52" s="29" t="s">
@@ -4152,10 +4149,10 @@
         <v>77</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="29" t="s">
@@ -4177,10 +4174,10 @@
         <v>78</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D54" s="29"/>
       <c r="E54" s="29" t="s">
@@ -4202,10 +4199,10 @@
         <v>79</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29" t="s">
@@ -4227,10 +4224,10 @@
         <v>80</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="29" t="s">
@@ -4252,10 +4249,10 @@
         <v>81</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="29" t="s">
@@ -4277,10 +4274,10 @@
         <v>82</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="29" t="s">
@@ -4302,10 +4299,10 @@
         <v>83</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29" t="s">
@@ -4327,10 +4324,10 @@
         <v>84</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="29" t="s">
@@ -4352,10 +4349,10 @@
         <v>85</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D61" s="29"/>
       <c r="E61" s="29" t="s">
@@ -4377,10 +4374,10 @@
         <v>86</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29" t="s">
@@ -4402,10 +4399,10 @@
         <v>87</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29" t="s">
@@ -4427,10 +4424,10 @@
         <v>88</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -4452,10 +4449,10 @@
         <v>89</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29" t="s">
@@ -4477,10 +4474,10 @@
         <v>90</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29" t="s">
@@ -4502,10 +4499,10 @@
         <v>91</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29" t="s">
@@ -4527,10 +4524,10 @@
         <v>92</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -4552,10 +4549,10 @@
         <v>93</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -4577,10 +4574,10 @@
         <v>94</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29" t="s">
@@ -4602,10 +4599,10 @@
         <v>95</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="29" t="s">
@@ -4627,10 +4624,10 @@
         <v>96</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D72" s="29"/>
       <c r="E72" s="29" t="s">
@@ -4655,7 +4652,7 @@
         <v>32</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29" t="s">
@@ -4680,7 +4677,7 @@
         <v>32</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29" t="s">
@@ -4705,7 +4702,7 @@
         <v>32</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D75" s="29"/>
       <c r="E75" s="29" t="s">
@@ -4727,10 +4724,10 @@
         <v>100</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="29" t="s">
@@ -4752,10 +4749,10 @@
         <v>101</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D77" s="29"/>
       <c r="E77" s="29" t="s">
@@ -4777,10 +4774,10 @@
         <v>102</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D78" s="29"/>
       <c r="E78" s="29" t="s">
@@ -4802,10 +4799,10 @@
         <v>103</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D79" s="29"/>
       <c r="E79" s="29" t="s">
@@ -4827,10 +4824,10 @@
         <v>104</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D80" s="29"/>
       <c r="E80" s="29" t="s">
@@ -4852,10 +4849,10 @@
         <v>105</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D81" s="29"/>
       <c r="E81" s="29" t="s">
@@ -4871,7 +4868,7 @@
         <v>17</v>
       </c>
       <c r="I81" s="31" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -4879,13 +4876,13 @@
         <v>106</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C82" s="31" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E82" s="29" t="s">
         <v>19</v>
@@ -4906,13 +4903,13 @@
         <v>107</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E83" s="29" t="s">
         <v>19</v>
@@ -4933,13 +4930,13 @@
         <v>108</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E84" s="29" t="s">
         <v>19</v>
@@ -4960,13 +4957,13 @@
         <v>109</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E85" s="29" t="s">
         <v>19</v>
@@ -4987,13 +4984,13 @@
         <v>110</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E86" s="29" t="s">
         <v>19</v>
@@ -5014,10 +5011,10 @@
         <v>111</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="29" t="s">
@@ -5036,13 +5033,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="22" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="29" t="s">
@@ -5064,10 +5061,10 @@
         <v>112</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29" t="s">
@@ -5086,13 +5083,13 @@
     </row>
     <row r="90" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="22" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="29" t="s">
@@ -5114,10 +5111,10 @@
         <v>113</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29" t="s">
@@ -5139,10 +5136,10 @@
         <v>114</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="29" t="s">
@@ -5164,10 +5161,10 @@
         <v>115</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="29" t="s">
@@ -5189,10 +5186,10 @@
         <v>116</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C94" s="31" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D94" s="29"/>
       <c r="E94" s="29" t="s">
@@ -5214,10 +5211,10 @@
         <v>117</v>
       </c>
       <c r="B95" s="30" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D95" s="29"/>
       <c r="E95" s="29" t="s">
@@ -5239,10 +5236,10 @@
         <v>118</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C96" s="31" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D96" s="29"/>
       <c r="E96" s="29" t="s">
@@ -5264,10 +5261,10 @@
         <v>119</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D97" s="29"/>
       <c r="E97" s="29" t="s">
@@ -5289,10 +5286,10 @@
         <v>120</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C98" s="31" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D98" s="29"/>
       <c r="E98" s="29" t="s">
@@ -5314,10 +5311,10 @@
         <v>121</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D99" s="29"/>
       <c r="E99" s="29" t="s">
@@ -5339,13 +5336,13 @@
         <v>122</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E100" s="29" t="s">
         <v>19</v>
@@ -5366,13 +5363,13 @@
         <v>123</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C101" s="31" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E101" s="29" t="s">
         <v>19</v>
@@ -5393,10 +5390,10 @@
         <v>124</v>
       </c>
       <c r="B102" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="29" t="s">
@@ -5418,10 +5415,10 @@
         <v>125</v>
       </c>
       <c r="B103" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C103" s="31" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D103" s="29"/>
       <c r="E103" s="29" t="s">
@@ -5443,10 +5440,10 @@
         <v>126</v>
       </c>
       <c r="B104" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29" t="s">
@@ -5465,16 +5462,16 @@
     </row>
     <row r="105" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A105" s="22" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D105" s="22" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="E105" s="29" t="s">
         <v>19</v>
@@ -5492,16 +5489,16 @@
     </row>
     <row r="106" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A106" s="22" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="B106" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D106" s="22" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="E106" s="29" t="s">
         <v>19</v>
@@ -5522,10 +5519,10 @@
         <v>127</v>
       </c>
       <c r="B107" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="29" t="s">
@@ -5547,10 +5544,10 @@
         <v>128</v>
       </c>
       <c r="B108" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="29" t="s">
@@ -5566,7 +5563,7 @@
         <v>17</v>
       </c>
       <c r="I108" s="31" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -5574,13 +5571,13 @@
         <v>129</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D109" s="29" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E109" s="29" t="s">
         <v>19</v>
@@ -5601,13 +5598,13 @@
         <v>130</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D110" s="29" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E110" s="29" t="s">
         <v>19</v>
@@ -5628,13 +5625,13 @@
         <v>131</v>
       </c>
       <c r="B111" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D111" s="29" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E111" s="29" t="s">
         <v>19</v>
@@ -5655,10 +5652,10 @@
         <v>132</v>
       </c>
       <c r="B112" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="29" t="s">
@@ -5680,10 +5677,10 @@
         <v>133</v>
       </c>
       <c r="B113" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D113" s="29"/>
       <c r="E113" s="29" t="s">
@@ -5705,10 +5702,10 @@
         <v>134</v>
       </c>
       <c r="B114" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C114" s="31" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="29" t="s">
@@ -5730,10 +5727,10 @@
         <v>135</v>
       </c>
       <c r="B115" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C115" s="31" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -5755,10 +5752,10 @@
         <v>136</v>
       </c>
       <c r="B116" s="24" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="29" t="s">
@@ -5774,7 +5771,7 @@
         <v>17</v>
       </c>
       <c r="I116" s="31" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
@@ -5782,10 +5779,10 @@
         <v>137</v>
       </c>
       <c r="B117" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C117" s="31" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="29" t="s">
@@ -5807,10 +5804,10 @@
         <v>138</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="29" t="s">
@@ -5832,10 +5829,10 @@
         <v>139</v>
       </c>
       <c r="B119" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C119" s="31" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="29" t="s">
@@ -5857,10 +5854,10 @@
         <v>140</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C120" s="31" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D120" s="29"/>
       <c r="E120" s="29" t="s">
@@ -5882,10 +5879,10 @@
         <v>141</v>
       </c>
       <c r="B121" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C121" s="31" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="29" t="s">
@@ -5907,10 +5904,10 @@
         <v>142</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C122" s="20" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="29" t="s">
@@ -5929,13 +5926,13 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="22" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C123" s="20" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -5957,10 +5954,10 @@
         <v>143</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C124" s="31" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="29" t="s">
@@ -5982,10 +5979,10 @@
         <v>144</v>
       </c>
       <c r="B125" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C125" s="31" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29" t="s">
@@ -6001,7 +5998,7 @@
         <v>17</v>
       </c>
       <c r="I125" s="31" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -6009,13 +6006,13 @@
         <v>145</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C126" s="31" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D126" s="29" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E126" s="29" t="s">
         <v>19</v>
@@ -6036,13 +6033,13 @@
         <v>146</v>
       </c>
       <c r="B127" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C127" s="31" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D127" s="29" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E127" s="29" t="s">
         <v>19</v>
@@ -6063,13 +6060,13 @@
         <v>147</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C128" s="31" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D128" s="29" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E128" s="29" t="s">
         <v>19</v>
@@ -6090,10 +6087,10 @@
         <v>148</v>
       </c>
       <c r="B129" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C129" s="31" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="29" t="s">
@@ -6115,10 +6112,10 @@
         <v>149</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C130" s="31" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="29" t="s">
@@ -6140,10 +6137,10 @@
         <v>150</v>
       </c>
       <c r="B131" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C131" s="31" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -6159,7 +6156,7 @@
         <v>17</v>
       </c>
       <c r="I131" s="31" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
@@ -6167,13 +6164,13 @@
         <v>151</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C132" s="31" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D132" s="29" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E132" s="29" t="s">
         <v>19</v>
@@ -6194,13 +6191,13 @@
         <v>152</v>
       </c>
       <c r="B133" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E133" s="29" t="s">
         <v>19</v>
@@ -6221,13 +6218,13 @@
         <v>153</v>
       </c>
       <c r="B134" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C134" s="31" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D134" s="29" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E134" s="29" t="s">
         <v>19</v>
@@ -6248,10 +6245,10 @@
         <v>154</v>
       </c>
       <c r="B135" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C135" s="31" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="29" t="s">
@@ -6273,10 +6270,10 @@
         <v>155</v>
       </c>
       <c r="B136" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C136" s="31" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="29" t="s">
@@ -6293,15 +6290,15 @@
       </c>
       <c r="I136" s="31"/>
     </row>
-    <row r="137" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A137" s="29" t="s">
         <v>156</v>
       </c>
       <c r="B137" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C137" s="31" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="29" t="s">
@@ -6316,22 +6313,22 @@
       <c r="H137" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I137" s="31" t="s">
-        <v>434</v>
+      <c r="I137" s="20" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A138" s="29" t="s">
-        <v>157</v>
+      <c r="A138" s="22" t="s">
+        <v>479</v>
       </c>
       <c r="B138" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C138" s="31" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D138" s="29" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E138" s="29" t="s">
         <v>19</v>
@@ -6348,17 +6345,17 @@
       <c r="I138" s="31"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A139" s="29" t="s">
-        <v>158</v>
+      <c r="A139" s="22" t="s">
+        <v>481</v>
       </c>
       <c r="B139" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C139" s="31" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D139" s="29" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E139" s="29" t="s">
         <v>19</v>
@@ -6374,19 +6371,17 @@
       </c>
       <c r="I139" s="31"/>
     </row>
-    <row r="140" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" s="29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B140" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C140" s="31" t="s">
-        <v>359</v>
-      </c>
-      <c r="D140" s="29" t="s">
-        <v>423</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="D140" s="29"/>
       <c r="E140" s="29" t="s">
         <v>19</v>
       </c>
@@ -6401,15 +6396,15 @@
       </c>
       <c r="I140" s="31"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A141" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B141" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C141" s="31" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="29" t="s">
@@ -6419,22 +6414,22 @@
         <v>3</v>
       </c>
       <c r="G141" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H141" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I141" s="31"/>
     </row>
-    <row r="142" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" s="29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B142" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C142" s="31" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="29" t="s">
@@ -6444,22 +6439,22 @@
         <v>3</v>
       </c>
       <c r="G142" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H142" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I142" s="31"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" s="29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B143" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C143" s="31" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -6469,22 +6464,22 @@
         <v>3</v>
       </c>
       <c r="G143" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H143" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I143" s="31"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A144" s="29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B144" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C144" s="31" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="29" t="s">
@@ -6494,24 +6489,28 @@
         <v>3</v>
       </c>
       <c r="G144" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H144" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I144" s="31"/>
-    </row>
-    <row r="145" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="I144" s="31" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B145" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>364</v>
-      </c>
-      <c r="D145" s="29"/>
+        <v>361</v>
+      </c>
+      <c r="D145" s="29" t="s">
+        <v>420</v>
+      </c>
       <c r="E145" s="29" t="s">
         <v>19</v>
       </c>
@@ -6522,24 +6521,22 @@
         <v>15</v>
       </c>
       <c r="H145" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I145" s="31" t="s">
-        <v>435</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I145" s="31"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" s="29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B146" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C146" s="31" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E146" s="29" t="s">
         <v>19</v>
@@ -6555,18 +6552,18 @@
       </c>
       <c r="I146" s="31"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B147" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C147" s="31" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D147" s="29" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E147" s="29" t="s">
         <v>19</v>
@@ -6582,19 +6579,17 @@
       </c>
       <c r="I147" s="31"/>
     </row>
-    <row r="148" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B148" s="30" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C148" s="31" t="s">
-        <v>367</v>
-      </c>
-      <c r="D148" s="29" t="s">
-        <v>424</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="D148" s="29"/>
       <c r="E148" s="29" t="s">
         <v>19</v>
       </c>
@@ -6609,40 +6604,40 @@
       </c>
       <c r="I148" s="31"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A149" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B149" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C149" s="31" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F149" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G149" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H149" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I149" s="31"/>
     </row>
-    <row r="150" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A150" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B150" s="30" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C150" s="31" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="29" t="s">
@@ -6652,22 +6647,22 @@
         <v>6</v>
       </c>
       <c r="G150" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H150" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I150" s="31"/>
     </row>
-    <row r="151" spans="1:9" ht="116" x14ac:dyDescent="0.35">
-      <c r="A151" s="29" t="s">
-        <v>170</v>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A151" s="22" t="s">
+        <v>168</v>
       </c>
       <c r="B151" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="C151" s="31" t="s">
-        <v>370</v>
+        <v>235</v>
+      </c>
+      <c r="C151" s="20" t="s">
+        <v>367</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="29" t="s">
@@ -6686,13 +6681,13 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" s="22" t="s">
-        <v>171</v>
+        <v>442</v>
       </c>
       <c r="B152" s="30" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C152" s="20" t="s">
-        <v>371</v>
+        <v>443</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="29" t="s">
@@ -6705,44 +6700,44 @@
         <v>15</v>
       </c>
       <c r="H152" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I152" s="31"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A153" s="22" t="s">
-        <v>447</v>
+      <c r="A153" s="29" t="s">
+        <v>169</v>
       </c>
       <c r="B153" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="C153" s="20" t="s">
-        <v>448</v>
+        <v>33</v>
+      </c>
+      <c r="C153" s="31" t="s">
+        <v>368</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F153" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G153" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H153" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I153" s="31"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A154" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B154" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C154" s="31" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="29" t="s">
@@ -6752,22 +6747,22 @@
         <v>3</v>
       </c>
       <c r="G154" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H154" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I154" s="31"/>
     </row>
-    <row r="155" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A155" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B155" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C155" s="31" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="29" t="s">
@@ -6786,13 +6781,13 @@
     </row>
     <row r="156" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A156" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B156" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C156" s="31" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="29" t="s">
@@ -6805,44 +6800,44 @@
         <v>15</v>
       </c>
       <c r="H156" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I156" s="31"/>
     </row>
-    <row r="157" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B157" s="30" t="s">
-        <v>33</v>
+        <v>236</v>
       </c>
       <c r="C157" s="31" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D157" s="29"/>
       <c r="E157" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F157" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G157" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H157" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I157" s="31"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A158" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B158" s="30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C158" s="31" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D158" s="29"/>
       <c r="E158" s="29" t="s">
@@ -6859,15 +6854,15 @@
       </c>
       <c r="I158" s="31"/>
     </row>
-    <row r="159" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B159" s="30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C159" s="31" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D159" s="29"/>
       <c r="E159" s="29" t="s">
@@ -6884,47 +6879,47 @@
       </c>
       <c r="I159" s="31"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A160" s="29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B160" s="30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C160" s="31" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D160" s="29"/>
       <c r="E160" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F160" s="29" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G160" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H160" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I160" s="31"/>
     </row>
     <row r="161" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A161" s="29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B161" s="30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C161" s="31" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D161" s="29"/>
       <c r="E161" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F161" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G161" s="29" t="s">
         <v>15</v>
@@ -6936,13 +6931,13 @@
     </row>
     <row r="162" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="29" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B162" s="30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C162" s="31" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D162" s="29"/>
       <c r="E162" s="29" t="s">
@@ -6961,13 +6956,13 @@
     </row>
     <row r="163" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="29" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B163" s="30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C163" s="31" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D163" s="29"/>
       <c r="E163" s="29" t="s">
@@ -6986,13 +6981,13 @@
     </row>
     <row r="164" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B164" s="30" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C164" s="31" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="29" t="s">
@@ -7002,22 +6997,22 @@
         <v>6</v>
       </c>
       <c r="G164" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H164" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I164" s="31"/>
     </row>
-    <row r="165" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" s="29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B165" s="30" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C165" s="31" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -7027,47 +7022,47 @@
         <v>6</v>
       </c>
       <c r="G165" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H165" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I165" s="31"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" s="29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B166" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C166" s="31" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D166" s="29"/>
       <c r="E166" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F166" s="29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G166" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H166" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I166" s="31"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A167" s="29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B167" s="30" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C167" s="31" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D167" s="29"/>
       <c r="E167" s="29" t="s">
@@ -7077,54 +7072,54 @@
         <v>7</v>
       </c>
       <c r="G167" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H167" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I167" s="31"/>
     </row>
-    <row r="168" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" s="29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B168" s="30" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D168" s="29"/>
       <c r="E168" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F168" s="29" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G168" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H168" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I168" s="31"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A169" s="29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B169" s="30" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D169" s="29"/>
       <c r="E169" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F169" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G169" s="29" t="s">
         <v>16</v>
@@ -7136,13 +7131,13 @@
     </row>
     <row r="170" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A170" s="29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B170" s="30" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C170" s="31" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D170" s="29"/>
       <c r="E170" s="29" t="s">
@@ -7152,47 +7147,47 @@
         <v>6</v>
       </c>
       <c r="G170" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H170" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I170" s="31"/>
     </row>
     <row r="171" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B171" s="30" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D171" s="29"/>
       <c r="E171" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F171" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G171" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H171" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I171" s="31"/>
     </row>
-    <row r="172" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A172" s="29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B172" s="30" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C172" s="31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D172" s="29"/>
       <c r="E172" s="29" t="s">
@@ -7202,29 +7197,29 @@
         <v>3</v>
       </c>
       <c r="G172" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H172" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I172" s="31"/>
     </row>
-    <row r="173" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B173" s="30" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F173" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G173" s="29" t="s">
         <v>15</v>
@@ -7236,38 +7231,38 @@
     </row>
     <row r="174" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="29" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B174" s="30" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D174" s="29"/>
       <c r="E174" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F174" s="29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G174" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H174" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I174" s="31"/>
     </row>
-    <row r="175" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A175" s="29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B175" s="30" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="29" t="s">
@@ -7277,22 +7272,22 @@
         <v>7</v>
       </c>
       <c r="G175" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H175" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I175" s="31"/>
     </row>
-    <row r="176" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" s="29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B176" s="30" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D176" s="29"/>
       <c r="E176" s="29" t="s">
@@ -7309,40 +7304,40 @@
       </c>
       <c r="I176" s="31"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A177" s="29" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B177" s="30" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D177" s="29"/>
       <c r="E177" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F177" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G177" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H177" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I177" s="31"/>
     </row>
-    <row r="178" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" s="29" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B178" s="30" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D178" s="29"/>
       <c r="E178" s="29" t="s">
@@ -7352,47 +7347,47 @@
         <v>6</v>
       </c>
       <c r="G178" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H178" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I178" s="31"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A179" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B179" s="30" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D179" s="29"/>
       <c r="E179" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F179" s="29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G179" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H179" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I179" s="31"/>
     </row>
-    <row r="180" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A180" s="29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B180" s="30" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D180" s="29"/>
       <c r="E180" s="29" t="s">
@@ -7402,47 +7397,47 @@
         <v>7</v>
       </c>
       <c r="G180" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H180" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I180" s="31"/>
     </row>
-    <row r="181" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B181" s="30" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D181" s="29"/>
       <c r="E181" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F181" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G181" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H181" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I181" s="31"/>
     </row>
-    <row r="182" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" ht="290" x14ac:dyDescent="0.35">
       <c r="A182" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B182" s="30" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D182" s="29"/>
       <c r="E182" s="29" t="s">
@@ -7452,22 +7447,22 @@
         <v>6</v>
       </c>
       <c r="G182" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H182" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I182" s="31"/>
     </row>
-    <row r="183" spans="1:9" ht="290" x14ac:dyDescent="0.35">
-      <c r="A183" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="B183" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="C183" s="31" t="s">
-        <v>401</v>
+    <row r="183" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A183" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B183" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="C183" s="20" t="s">
+        <v>398</v>
       </c>
       <c r="D183" s="29"/>
       <c r="E183" s="29" t="s">
@@ -7484,15 +7479,15 @@
       </c>
       <c r="I183" s="31"/>
     </row>
-    <row r="184" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" s="22" t="s">
-        <v>202</v>
+        <v>444</v>
       </c>
       <c r="B184" s="24" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C184" s="20" t="s">
-        <v>402</v>
+        <v>445</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="29" t="s">
@@ -7509,15 +7504,15 @@
       </c>
       <c r="I184" s="31"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A185" s="22" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B185" s="24" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C185" s="20" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D185" s="29"/>
       <c r="E185" s="29" t="s">
@@ -7535,39 +7530,39 @@
       <c r="I185" s="31"/>
     </row>
     <row r="186" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A186" s="22" t="s">
-        <v>451</v>
-      </c>
-      <c r="B186" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="C186" s="20" t="s">
-        <v>452</v>
+      <c r="A186" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B186" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="C186" s="31" t="s">
+        <v>399</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F186" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G186" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H186" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I186" s="31"/>
     </row>
-    <row r="187" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" s="29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B187" s="30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="29" t="s">
@@ -7577,22 +7572,22 @@
         <v>3</v>
       </c>
       <c r="G187" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H187" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I187" s="31"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A188" s="29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B188" s="30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="29" t="s">
@@ -7609,22 +7604,22 @@
       </c>
       <c r="I188" s="31"/>
     </row>
-    <row r="189" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A189" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B189" s="30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D189" s="29"/>
       <c r="E189" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F189" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G189" s="29" t="s">
         <v>15</v>
@@ -7636,38 +7631,38 @@
     </row>
     <row r="190" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="29" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B190" s="30" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D190" s="29"/>
       <c r="E190" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F190" s="29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G190" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H190" s="29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I190" s="31"/>
     </row>
-    <row r="191" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A191" s="29" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B191" s="30" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D191" s="29"/>
       <c r="E191" s="29" t="s">
@@ -7677,22 +7672,22 @@
         <v>7</v>
       </c>
       <c r="G191" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H191" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I191" s="31"/>
     </row>
-    <row r="192" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" s="29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B192" s="30" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D192" s="29"/>
       <c r="E192" s="29" t="s">
@@ -7709,40 +7704,40 @@
       </c>
       <c r="I192" s="31"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="29" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B193" s="30" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D193" s="29"/>
       <c r="E193" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F193" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G193" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H193" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I193" s="31"/>
     </row>
-    <row r="194" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" s="29" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B194" s="30" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="29" t="s">
@@ -7752,47 +7747,47 @@
         <v>6</v>
       </c>
       <c r="G194" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H194" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I194" s="31"/>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" s="29" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B195" s="30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D195" s="29"/>
       <c r="E195" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F195" s="29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G195" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H195" s="29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I195" s="31"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A196" s="29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B196" s="30" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -7802,22 +7797,22 @@
         <v>7</v>
       </c>
       <c r="G196" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H196" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I196" s="31"/>
     </row>
-    <row r="197" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A197" s="29" t="s">
-        <v>213</v>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A197" s="22" t="s">
+        <v>211</v>
       </c>
       <c r="B197" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="C197" s="31" t="s">
-        <v>413</v>
+        <v>248</v>
+      </c>
+      <c r="C197" s="20" t="s">
+        <v>448</v>
       </c>
       <c r="D197" s="29"/>
       <c r="E197" s="29" t="s">
@@ -7836,13 +7831,13 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" s="22" t="s">
-        <v>214</v>
+        <v>449</v>
       </c>
       <c r="B198" s="30" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -7859,15 +7854,15 @@
       </c>
       <c r="I198" s="31"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A199" s="22" t="s">
-        <v>454</v>
+    <row r="199" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A199" s="29" t="s">
+        <v>212</v>
       </c>
       <c r="B199" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="C199" s="20" t="s">
-        <v>455</v>
+        <v>248</v>
+      </c>
+      <c r="C199" s="31" t="s">
+        <v>410</v>
       </c>
       <c r="D199" s="29"/>
       <c r="E199" s="29" t="s">
@@ -7886,38 +7881,38 @@
     </row>
     <row r="200" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B200" s="30" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D200" s="29"/>
       <c r="E200" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F200" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G200" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H200" s="29" t="s">
         <v>18</v>
       </c>
       <c r="I200" s="31"/>
     </row>
-    <row r="201" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A201" s="29" t="s">
-        <v>216</v>
+    <row r="201" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A201" s="22" t="s">
+        <v>214</v>
       </c>
       <c r="B201" s="30" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -7927,47 +7922,47 @@
         <v>6</v>
       </c>
       <c r="G201" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H201" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I201" s="31"/>
     </row>
-    <row r="202" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A202" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="B202" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="C202" s="31" t="s">
-        <v>416</v>
+        <v>452</v>
+      </c>
+      <c r="B202" s="24" t="s">
+        <v>453</v>
+      </c>
+      <c r="C202" s="20" t="s">
+        <v>454</v>
       </c>
       <c r="D202" s="29"/>
       <c r="E202" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F202" s="29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G202" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H202" s="29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I202" s="31"/>
     </row>
-    <row r="203" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" s="22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B203" s="24" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C203" s="20" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D203" s="29"/>
       <c r="E203" s="29" t="s">
@@ -7977,7 +7972,7 @@
         <v>7</v>
       </c>
       <c r="G203" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H203" s="29" t="s">
         <v>18</v>
@@ -7986,13 +7981,13 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" s="22" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B204" s="24" t="s">
         <v>458</v>
       </c>
       <c r="C204" s="20" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D204" s="29"/>
       <c r="E204" s="29" t="s">
@@ -8009,15 +8004,15 @@
       </c>
       <c r="I204" s="31"/>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A205" s="22" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B205" s="24" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C205" s="20" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D205" s="29"/>
       <c r="E205" s="29" t="s">
@@ -8034,69 +8029,69 @@
       </c>
       <c r="I205" s="31"/>
     </row>
-    <row r="206" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A206" s="22" t="s">
-        <v>465</v>
-      </c>
-      <c r="B206" s="24" t="s">
-        <v>463</v>
+        <v>45</v>
+      </c>
+      <c r="B206" s="32">
+        <v>7</v>
       </c>
       <c r="C206" s="20" t="s">
-        <v>466</v>
-      </c>
-      <c r="D206" s="29"/>
-      <c r="E206" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F206" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G206" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H206" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I206" s="31"/>
-    </row>
-    <row r="207" spans="1:9" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A207" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B207" s="32">
-        <v>7</v>
-      </c>
-      <c r="C207" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="D207" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="E207" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D206" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="E206" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F207" s="22" t="s">
+      <c r="F206" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G207" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H207" s="22" t="s">
+      <c r="G206" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H206" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I207" s="24" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I206" s="24" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A207" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="B207" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="C207" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="D207" s="29"/>
+      <c r="E207" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F207" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G207" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H207" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I207" s="31"/>
+    </row>
+    <row r="208" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A208" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B208" s="30" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C208" s="31" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -8113,17 +8108,19 @@
       </c>
       <c r="I208" s="31"/>
     </row>
-    <row r="209" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A209" s="29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B209" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="C209" s="31" t="s">
-        <v>439</v>
-      </c>
-      <c r="D209" s="29"/>
+        <v>250</v>
+      </c>
+      <c r="C209" s="20" t="s">
+        <v>432</v>
+      </c>
+      <c r="D209" s="24" t="s">
+        <v>431</v>
+      </c>
       <c r="E209" s="29" t="s">
         <v>22</v>
       </c>
@@ -8131,82 +8128,50 @@
         <v>3</v>
       </c>
       <c r="G209" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H209" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I209" s="31"/>
-    </row>
-    <row r="210" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="I209" s="31" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A210" s="29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B210" s="30" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C210" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="D210" s="24" t="s">
-        <v>436</v>
-      </c>
+        <v>451</v>
+      </c>
+      <c r="D210" s="29"/>
       <c r="E210" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F210" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G210" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H210" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I210" s="31" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A211" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="B211" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="C211" s="20" t="s">
-        <v>456</v>
-      </c>
-      <c r="D211" s="29"/>
-      <c r="E211" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F211" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G211" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H211" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I211" s="31"/>
+        <v>18</v>
+      </c>
+      <c r="I210" s="31"/>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A211" s="3"/>
+      <c r="B211" s="10"/>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" s="3"/>
       <c r="B212" s="10"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A213" s="3"/>
-      <c r="B213" s="10"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -8214,53 +8179,58 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A208:I211 A20:I21 A207:H207 A22:H113 I22:I207 A33:I206">
-    <cfRule type="expression" dxfId="26" priority="53">
+  <conditionalFormatting sqref="A207:I210 A20:I21 A206:H206 A22:H113 I22:I206 A33:I205">
+    <cfRule type="expression" dxfId="7" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="54">
+    <cfRule type="expression" dxfId="6" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="61">
+    <cfRule type="expression" dxfId="5" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A208:I211 A20:I21 A207:H207 A22:H113 I22:I207 A33:I206">
-    <cfRule type="expression" dxfId="23" priority="7">
+  <conditionalFormatting sqref="A207:I210 A20:I21 A206:H206 A22:H113 I22:I206 A33:I205">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F211">
-    <cfRule type="expression" dxfId="20" priority="13">
+  <conditionalFormatting sqref="F20:F210">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F211" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F210" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E211" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E210" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G211" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G210" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H211" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H210" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8270,7 +8240,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B2 B4:B9 B10:B21 B88:B90 B22:B87 B106:B186 B206:B213 B187:B205 B91:B105 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B2 B4:B9 B10:B21 B88:B90 B22:B87 B106:B139 B205:B212 B186:B204 B91:B105 C3 B140:B185" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -8280,18 +8250,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8344,14 +8314,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -8361,6 +8323,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>